<commit_message>
add backprop for conv, bn, relu, maxpool, and linear
</commit_message>
<xml_diff>
--- a/outputs/torch/resnet50.xlsx
+++ b/outputs/torch/resnet50.xlsx
@@ -97,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -117,11 +117,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -510,7 +507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W184"/>
+  <dimension ref="A1:X184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -519,6 +516,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
+    <col width="1" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
@@ -577,118 +575,124 @@
         </is>
       </c>
       <c r="V1" s="11" t="n"/>
-      <c r="W1" s="12" t="n"/>
+      <c r="W1" s="11" t="n"/>
+      <c r="X1" s="12" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="inlineStr"/>
-      <c r="B2" s="13" t="inlineStr">
+      <c r="A2" s="10" t="inlineStr"/>
+      <c r="B2" s="10" t="inlineStr">
         <is>
           <t>L0</t>
         </is>
       </c>
-      <c r="C2" s="13" t="inlineStr">
+      <c r="C2" s="10" t="inlineStr">
         <is>
           <t>L1</t>
         </is>
       </c>
-      <c r="D2" s="13" t="inlineStr">
+      <c r="D2" s="10" t="inlineStr">
         <is>
           <t>L2</t>
         </is>
       </c>
-      <c r="E2" s="13" t="inlineStr">
+      <c r="E2" s="10" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
       </c>
-      <c r="F2" s="13" t="inlineStr">
+      <c r="F2" s="10" t="inlineStr">
         <is>
           <t>I1</t>
         </is>
       </c>
-      <c r="G2" s="13" t="inlineStr">
+      <c r="G2" s="10" t="inlineStr">
         <is>
           <t>I2</t>
         </is>
       </c>
-      <c r="H2" s="13" t="inlineStr">
+      <c r="H2" s="10" t="inlineStr">
         <is>
           <t>I3</t>
         </is>
       </c>
-      <c r="I2" s="13" t="inlineStr">
+      <c r="I2" s="10" t="inlineStr">
         <is>
           <t>O1</t>
         </is>
       </c>
-      <c r="J2" s="13" t="inlineStr">
+      <c r="J2" s="10" t="inlineStr">
         <is>
           <t>O2</t>
         </is>
       </c>
-      <c r="K2" s="13" t="inlineStr">
+      <c r="K2" s="10" t="inlineStr">
         <is>
           <t>O3</t>
         </is>
       </c>
-      <c r="L2" s="13" t="inlineStr">
+      <c r="L2" s="10" t="inlineStr">
         <is>
           <t>k1</t>
         </is>
       </c>
-      <c r="M2" s="13" t="inlineStr">
+      <c r="M2" s="10" t="inlineStr">
         <is>
           <t>k2</t>
         </is>
       </c>
-      <c r="N2" s="13" t="inlineStr">
+      <c r="N2" s="10" t="inlineStr">
         <is>
           <t>s1</t>
         </is>
       </c>
-      <c r="O2" s="13" t="inlineStr">
+      <c r="O2" s="10" t="inlineStr">
         <is>
           <t>s2</t>
         </is>
       </c>
-      <c r="P2" s="13" t="inlineStr">
+      <c r="P2" s="10" t="inlineStr">
         <is>
           <t>p1</t>
         </is>
       </c>
-      <c r="Q2" s="13" t="inlineStr">
+      <c r="Q2" s="10" t="inlineStr">
         <is>
           <t>p2</t>
         </is>
       </c>
-      <c r="R2" s="13" t="inlineStr">
+      <c r="R2" s="10" t="inlineStr">
         <is>
           <t>Input</t>
         </is>
       </c>
-      <c r="S2" s="13" t="inlineStr">
+      <c r="S2" s="10" t="inlineStr">
         <is>
           <t>Output</t>
         </is>
       </c>
-      <c r="T2" s="13" t="inlineStr">
+      <c r="T2" s="10" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="U2" s="13" t="inlineStr">
+      <c r="U2" s="10" t="inlineStr">
         <is>
           <t>GEMM</t>
         </is>
       </c>
-      <c r="V2" s="13" t="inlineStr">
+      <c r="V2" s="10" t="inlineStr">
         <is>
           <t>ElemWise</t>
         </is>
       </c>
-      <c r="W2" s="13" t="inlineStr">
+      <c r="W2" s="10" t="inlineStr">
         <is>
           <t>Activation</t>
+        </is>
+      </c>
+      <c r="X2" s="10" t="inlineStr">
+        <is>
+          <t>BackProp</t>
         </is>
       </c>
     </row>
@@ -750,10 +754,13 @@
         <v>9408</v>
       </c>
       <c r="U3" s="8" t="n">
-        <v>118013952</v>
+        <v>472055808</v>
       </c>
       <c r="V3" s="8" t="n"/>
       <c r="W3" s="8" t="n"/>
+      <c r="X3" s="8" t="n">
+        <v>472055808</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="7" t="n">
@@ -805,6 +812,9 @@
         <v>1605632</v>
       </c>
       <c r="W4" s="8" t="n"/>
+      <c r="X4" s="8" t="n">
+        <v>1605632</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="n">
@@ -854,6 +864,9 @@
       <c r="W5" s="8" t="n">
         <v>802816</v>
       </c>
+      <c r="X5" s="8" t="n">
+        <v>802816</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="n">
@@ -911,6 +924,9 @@
         <v>1605632</v>
       </c>
       <c r="W6" s="8" t="n"/>
+      <c r="X6" s="8" t="n">
+        <v>2517630976</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="n">
@@ -958,6 +974,7 @@
       <c r="U7" s="8" t="n"/>
       <c r="V7" s="8" t="n"/>
       <c r="W7" s="8" t="n"/>
+      <c r="X7" s="8" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="7" t="n">
@@ -1007,6 +1024,7 @@
       <c r="U8" s="8" t="n"/>
       <c r="V8" s="8" t="n"/>
       <c r="W8" s="8" t="n"/>
+      <c r="X8" s="8" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="7" t="n">
@@ -1070,6 +1088,9 @@
       </c>
       <c r="V9" s="8" t="n"/>
       <c r="W9" s="8" t="n"/>
+      <c r="X9" s="8" t="n">
+        <v>12845056</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="n">
@@ -1121,6 +1142,9 @@
         <v>401408</v>
       </c>
       <c r="W10" s="8" t="n"/>
+      <c r="X10" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="n">
@@ -1170,6 +1194,9 @@
       <c r="W11" s="8" t="n">
         <v>200704</v>
       </c>
+      <c r="X11" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="7" t="n">
@@ -1233,6 +1260,9 @@
       </c>
       <c r="V12" s="8" t="n"/>
       <c r="W12" s="8" t="n"/>
+      <c r="X12" s="8" t="n">
+        <v>115605504</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="7" t="n">
@@ -1284,6 +1314,9 @@
         <v>401408</v>
       </c>
       <c r="W13" s="8" t="n"/>
+      <c r="X13" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="7" t="n">
@@ -1333,6 +1366,9 @@
       <c r="W14" s="8" t="n">
         <v>200704</v>
       </c>
+      <c r="X14" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="7" t="n">
@@ -1396,6 +1432,9 @@
       </c>
       <c r="V15" s="8" t="n"/>
       <c r="W15" s="8" t="n"/>
+      <c r="X15" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="7" t="n">
@@ -1447,6 +1486,9 @@
         <v>1605632</v>
       </c>
       <c r="W16" s="8" t="n"/>
+      <c r="X16" s="8" t="n">
+        <v>1605632</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="7" t="n">
@@ -1494,6 +1536,7 @@
       <c r="U17" s="8" t="n"/>
       <c r="V17" s="8" t="n"/>
       <c r="W17" s="8" t="n"/>
+      <c r="X17" s="8" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="7" t="n">
@@ -1557,6 +1600,9 @@
       </c>
       <c r="V18" s="8" t="n"/>
       <c r="W18" s="8" t="n"/>
+      <c r="X18" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="n">
@@ -1608,6 +1654,9 @@
         <v>1605632</v>
       </c>
       <c r="W19" s="8" t="n"/>
+      <c r="X19" s="8" t="n">
+        <v>1605632</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="7" t="n">
@@ -1657,6 +1706,9 @@
       <c r="W20" s="8" t="n">
         <v>802816</v>
       </c>
+      <c r="X20" s="8" t="n">
+        <v>802816</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="7" t="n">
@@ -1706,6 +1758,7 @@
       <c r="U21" s="8" t="n"/>
       <c r="V21" s="8" t="n"/>
       <c r="W21" s="8" t="n"/>
+      <c r="X21" s="8" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="7" t="n">
@@ -1769,6 +1822,9 @@
       </c>
       <c r="V22" s="8" t="n"/>
       <c r="W22" s="8" t="n"/>
+      <c r="X22" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="7" t="n">
@@ -1820,6 +1876,9 @@
         <v>401408</v>
       </c>
       <c r="W23" s="8" t="n"/>
+      <c r="X23" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="7" t="n">
@@ -1869,6 +1928,9 @@
       <c r="W24" s="8" t="n">
         <v>200704</v>
       </c>
+      <c r="X24" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="7" t="n">
@@ -1932,6 +1994,9 @@
       </c>
       <c r="V25" s="8" t="n"/>
       <c r="W25" s="8" t="n"/>
+      <c r="X25" s="8" t="n">
+        <v>115605504</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="7" t="n">
@@ -1983,6 +2048,9 @@
         <v>401408</v>
       </c>
       <c r="W26" s="8" t="n"/>
+      <c r="X26" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="7" t="n">
@@ -2032,6 +2100,9 @@
       <c r="W27" s="8" t="n">
         <v>200704</v>
       </c>
+      <c r="X27" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="7" t="n">
@@ -2095,6 +2166,9 @@
       </c>
       <c r="V28" s="8" t="n"/>
       <c r="W28" s="8" t="n"/>
+      <c r="X28" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="7" t="n">
@@ -2146,6 +2220,9 @@
         <v>1605632</v>
       </c>
       <c r="W29" s="8" t="n"/>
+      <c r="X29" s="8" t="n">
+        <v>1605632</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="7" t="n">
@@ -2195,6 +2272,9 @@
       <c r="W30" s="8" t="n">
         <v>802816</v>
       </c>
+      <c r="X30" s="8" t="n">
+        <v>802816</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="7" t="n">
@@ -2244,6 +2324,7 @@
       <c r="U31" s="8" t="n"/>
       <c r="V31" s="8" t="n"/>
       <c r="W31" s="8" t="n"/>
+      <c r="X31" s="8" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="7" t="n">
@@ -2307,6 +2388,9 @@
       </c>
       <c r="V32" s="8" t="n"/>
       <c r="W32" s="8" t="n"/>
+      <c r="X32" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="7" t="n">
@@ -2358,6 +2442,9 @@
         <v>401408</v>
       </c>
       <c r="W33" s="8" t="n"/>
+      <c r="X33" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="7" t="n">
@@ -2407,6 +2494,9 @@
       <c r="W34" s="8" t="n">
         <v>200704</v>
       </c>
+      <c r="X34" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="7" t="n">
@@ -2470,6 +2560,9 @@
       </c>
       <c r="V35" s="8" t="n"/>
       <c r="W35" s="8" t="n"/>
+      <c r="X35" s="8" t="n">
+        <v>115605504</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="7" t="n">
@@ -2521,6 +2614,9 @@
         <v>401408</v>
       </c>
       <c r="W36" s="8" t="n"/>
+      <c r="X36" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="7" t="n">
@@ -2570,6 +2666,9 @@
       <c r="W37" s="8" t="n">
         <v>200704</v>
       </c>
+      <c r="X37" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="7" t="n">
@@ -2633,6 +2732,9 @@
       </c>
       <c r="V38" s="8" t="n"/>
       <c r="W38" s="8" t="n"/>
+      <c r="X38" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="7" t="n">
@@ -2684,6 +2786,9 @@
         <v>1605632</v>
       </c>
       <c r="W39" s="8" t="n"/>
+      <c r="X39" s="8" t="n">
+        <v>1605632</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="7" t="n">
@@ -2733,6 +2838,9 @@
       <c r="W40" s="8" t="n">
         <v>802816</v>
       </c>
+      <c r="X40" s="8" t="n">
+        <v>802816</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="7" t="n">
@@ -2780,6 +2888,7 @@
       <c r="U41" s="8" t="n"/>
       <c r="V41" s="8" t="n"/>
       <c r="W41" s="8" t="n"/>
+      <c r="X41" s="8" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="7" t="n">
@@ -2829,6 +2938,7 @@
       <c r="U42" s="8" t="n"/>
       <c r="V42" s="8" t="n"/>
       <c r="W42" s="8" t="n"/>
+      <c r="X42" s="8" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="7" t="n">
@@ -2892,6 +3002,9 @@
       </c>
       <c r="V43" s="8" t="n"/>
       <c r="W43" s="8" t="n"/>
+      <c r="X43" s="8" t="n">
+        <v>102760448</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="7" t="n">
@@ -2943,6 +3056,9 @@
         <v>802816</v>
       </c>
       <c r="W44" s="8" t="n"/>
+      <c r="X44" s="8" t="n">
+        <v>802816</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="7" t="n">
@@ -2992,6 +3108,9 @@
       <c r="W45" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="X45" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="7" t="n">
@@ -3051,10 +3170,13 @@
         <v>147456</v>
       </c>
       <c r="U46" s="8" t="n">
-        <v>115605504</v>
+        <v>462422016</v>
       </c>
       <c r="V46" s="8" t="n"/>
       <c r="W46" s="8" t="n"/>
+      <c r="X46" s="8" t="n">
+        <v>462422016</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="7" t="n">
@@ -3106,6 +3228,9 @@
         <v>200704</v>
       </c>
       <c r="W47" s="8" t="n"/>
+      <c r="X47" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="7" t="n">
@@ -3155,6 +3280,9 @@
       <c r="W48" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="X48" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="7" t="n">
@@ -3218,6 +3346,9 @@
       </c>
       <c r="V49" s="8" t="n"/>
       <c r="W49" s="8" t="n"/>
+      <c r="X49" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="7" t="n">
@@ -3269,6 +3400,9 @@
         <v>802816</v>
       </c>
       <c r="W50" s="8" t="n"/>
+      <c r="X50" s="8" t="n">
+        <v>802816</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="7" t="n">
@@ -3316,6 +3450,7 @@
       <c r="U51" s="8" t="n"/>
       <c r="V51" s="8" t="n"/>
       <c r="W51" s="8" t="n"/>
+      <c r="X51" s="8" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="7" t="n">
@@ -3375,10 +3510,13 @@
         <v>131072</v>
       </c>
       <c r="U52" s="8" t="n">
-        <v>102760448</v>
+        <v>411041792</v>
       </c>
       <c r="V52" s="8" t="n"/>
       <c r="W52" s="8" t="n"/>
+      <c r="X52" s="8" t="n">
+        <v>411041792</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="7" t="n">
@@ -3430,6 +3568,9 @@
         <v>802816</v>
       </c>
       <c r="W53" s="8" t="n"/>
+      <c r="X53" s="8" t="n">
+        <v>802816</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="7" t="n">
@@ -3479,6 +3620,9 @@
       <c r="W54" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="X54" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="7" t="n">
@@ -3528,6 +3672,7 @@
       <c r="U55" s="8" t="n"/>
       <c r="V55" s="8" t="n"/>
       <c r="W55" s="8" t="n"/>
+      <c r="X55" s="8" t="n"/>
     </row>
     <row r="56">
       <c r="A56" s="7" t="n">
@@ -3591,6 +3736,9 @@
       </c>
       <c r="V56" s="8" t="n"/>
       <c r="W56" s="8" t="n"/>
+      <c r="X56" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="7" t="n">
@@ -3642,6 +3790,9 @@
         <v>200704</v>
       </c>
       <c r="W57" s="8" t="n"/>
+      <c r="X57" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="7" t="n">
@@ -3691,6 +3842,9 @@
       <c r="W58" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="X58" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="7" t="n">
@@ -3754,6 +3908,9 @@
       </c>
       <c r="V59" s="8" t="n"/>
       <c r="W59" s="8" t="n"/>
+      <c r="X59" s="8" t="n">
+        <v>115605504</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="7" t="n">
@@ -3805,6 +3962,9 @@
         <v>200704</v>
       </c>
       <c r="W60" s="8" t="n"/>
+      <c r="X60" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="7" t="n">
@@ -3854,6 +4014,9 @@
       <c r="W61" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="X61" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="7" t="n">
@@ -3917,6 +4080,9 @@
       </c>
       <c r="V62" s="8" t="n"/>
       <c r="W62" s="8" t="n"/>
+      <c r="X62" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="7" t="n">
@@ -3968,6 +4134,9 @@
         <v>802816</v>
       </c>
       <c r="W63" s="8" t="n"/>
+      <c r="X63" s="8" t="n">
+        <v>802816</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="7" t="n">
@@ -4017,6 +4186,9 @@
       <c r="W64" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="X64" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="7" t="n">
@@ -4066,6 +4238,7 @@
       <c r="U65" s="8" t="n"/>
       <c r="V65" s="8" t="n"/>
       <c r="W65" s="8" t="n"/>
+      <c r="X65" s="8" t="n"/>
     </row>
     <row r="66">
       <c r="A66" s="7" t="n">
@@ -4129,6 +4302,9 @@
       </c>
       <c r="V66" s="8" t="n"/>
       <c r="W66" s="8" t="n"/>
+      <c r="X66" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="7" t="n">
@@ -4180,6 +4356,9 @@
         <v>200704</v>
       </c>
       <c r="W67" s="8" t="n"/>
+      <c r="X67" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="7" t="n">
@@ -4229,6 +4408,9 @@
       <c r="W68" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="X68" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="7" t="n">
@@ -4292,6 +4474,9 @@
       </c>
       <c r="V69" s="8" t="n"/>
       <c r="W69" s="8" t="n"/>
+      <c r="X69" s="8" t="n">
+        <v>115605504</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="7" t="n">
@@ -4343,6 +4528,9 @@
         <v>200704</v>
       </c>
       <c r="W70" s="8" t="n"/>
+      <c r="X70" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="7" t="n">
@@ -4392,6 +4580,9 @@
       <c r="W71" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="X71" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="7" t="n">
@@ -4455,6 +4646,9 @@
       </c>
       <c r="V72" s="8" t="n"/>
       <c r="W72" s="8" t="n"/>
+      <c r="X72" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="7" t="n">
@@ -4506,6 +4700,9 @@
         <v>802816</v>
       </c>
       <c r="W73" s="8" t="n"/>
+      <c r="X73" s="8" t="n">
+        <v>802816</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="7" t="n">
@@ -4555,6 +4752,9 @@
       <c r="W74" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="X74" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="7" t="n">
@@ -4604,6 +4804,7 @@
       <c r="U75" s="8" t="n"/>
       <c r="V75" s="8" t="n"/>
       <c r="W75" s="8" t="n"/>
+      <c r="X75" s="8" t="n"/>
     </row>
     <row r="76">
       <c r="A76" s="7" t="n">
@@ -4667,6 +4868,9 @@
       </c>
       <c r="V76" s="8" t="n"/>
       <c r="W76" s="8" t="n"/>
+      <c r="X76" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="7" t="n">
@@ -4718,6 +4922,9 @@
         <v>200704</v>
       </c>
       <c r="W77" s="8" t="n"/>
+      <c r="X77" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="7" t="n">
@@ -4767,6 +4974,9 @@
       <c r="W78" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="X78" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="7" t="n">
@@ -4830,6 +5040,9 @@
       </c>
       <c r="V79" s="8" t="n"/>
       <c r="W79" s="8" t="n"/>
+      <c r="X79" s="8" t="n">
+        <v>115605504</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="7" t="n">
@@ -4881,6 +5094,9 @@
         <v>200704</v>
       </c>
       <c r="W80" s="8" t="n"/>
+      <c r="X80" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="7" t="n">
@@ -4930,6 +5146,9 @@
       <c r="W81" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="X81" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="7" t="n">
@@ -4993,6 +5212,9 @@
       </c>
       <c r="V82" s="8" t="n"/>
       <c r="W82" s="8" t="n"/>
+      <c r="X82" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="7" t="n">
@@ -5044,6 +5266,9 @@
         <v>802816</v>
       </c>
       <c r="W83" s="8" t="n"/>
+      <c r="X83" s="8" t="n">
+        <v>802816</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="7" t="n">
@@ -5093,6 +5318,9 @@
       <c r="W84" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="X84" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="7" t="n">
@@ -5140,6 +5368,7 @@
       <c r="U85" s="8" t="n"/>
       <c r="V85" s="8" t="n"/>
       <c r="W85" s="8" t="n"/>
+      <c r="X85" s="8" t="n"/>
     </row>
     <row r="86">
       <c r="A86" s="7" t="n">
@@ -5189,6 +5418,7 @@
       <c r="U86" s="8" t="n"/>
       <c r="V86" s="8" t="n"/>
       <c r="W86" s="8" t="n"/>
+      <c r="X86" s="8" t="n"/>
     </row>
     <row r="87">
       <c r="A87" s="7" t="n">
@@ -5252,6 +5482,9 @@
       </c>
       <c r="V87" s="8" t="n"/>
       <c r="W87" s="8" t="n"/>
+      <c r="X87" s="8" t="n">
+        <v>102760448</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="7" t="n">
@@ -5303,6 +5536,9 @@
         <v>401408</v>
       </c>
       <c r="W88" s="8" t="n"/>
+      <c r="X88" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="7" t="n">
@@ -5352,6 +5588,9 @@
       <c r="W89" s="8" t="n">
         <v>200704</v>
       </c>
+      <c r="X89" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="7" t="n">
@@ -5411,10 +5650,13 @@
         <v>589824</v>
       </c>
       <c r="U90" s="8" t="n">
-        <v>115605504</v>
+        <v>462422016</v>
       </c>
       <c r="V90" s="8" t="n"/>
       <c r="W90" s="8" t="n"/>
+      <c r="X90" s="8" t="n">
+        <v>462422016</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="7" t="n">
@@ -5466,6 +5708,9 @@
         <v>100352</v>
       </c>
       <c r="W91" s="8" t="n"/>
+      <c r="X91" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="7" t="n">
@@ -5515,6 +5760,9 @@
       <c r="W92" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="X92" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="7" t="n">
@@ -5578,6 +5826,9 @@
       </c>
       <c r="V93" s="8" t="n"/>
       <c r="W93" s="8" t="n"/>
+      <c r="X93" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="7" t="n">
@@ -5629,6 +5880,9 @@
         <v>401408</v>
       </c>
       <c r="W94" s="8" t="n"/>
+      <c r="X94" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="7" t="n">
@@ -5676,6 +5930,7 @@
       <c r="U95" s="8" t="n"/>
       <c r="V95" s="8" t="n"/>
       <c r="W95" s="8" t="n"/>
+      <c r="X95" s="8" t="n"/>
     </row>
     <row r="96">
       <c r="A96" s="7" t="n">
@@ -5735,10 +5990,13 @@
         <v>524288</v>
       </c>
       <c r="U96" s="8" t="n">
-        <v>102760448</v>
+        <v>411041792</v>
       </c>
       <c r="V96" s="8" t="n"/>
       <c r="W96" s="8" t="n"/>
+      <c r="X96" s="8" t="n">
+        <v>411041792</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="7" t="n">
@@ -5790,6 +6048,9 @@
         <v>401408</v>
       </c>
       <c r="W97" s="8" t="n"/>
+      <c r="X97" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="7" t="n">
@@ -5839,6 +6100,9 @@
       <c r="W98" s="8" t="n">
         <v>200704</v>
       </c>
+      <c r="X98" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="7" t="n">
@@ -5888,6 +6152,7 @@
       <c r="U99" s="8" t="n"/>
       <c r="V99" s="8" t="n"/>
       <c r="W99" s="8" t="n"/>
+      <c r="X99" s="8" t="n"/>
     </row>
     <row r="100">
       <c r="A100" s="7" t="n">
@@ -5951,6 +6216,9 @@
       </c>
       <c r="V100" s="8" t="n"/>
       <c r="W100" s="8" t="n"/>
+      <c r="X100" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="7" t="n">
@@ -6002,6 +6270,9 @@
         <v>100352</v>
       </c>
       <c r="W101" s="8" t="n"/>
+      <c r="X101" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="7" t="n">
@@ -6051,6 +6322,9 @@
       <c r="W102" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="X102" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="7" t="n">
@@ -6114,6 +6388,9 @@
       </c>
       <c r="V103" s="8" t="n"/>
       <c r="W103" s="8" t="n"/>
+      <c r="X103" s="8" t="n">
+        <v>115605504</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="7" t="n">
@@ -6165,6 +6442,9 @@
         <v>100352</v>
       </c>
       <c r="W104" s="8" t="n"/>
+      <c r="X104" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="7" t="n">
@@ -6214,6 +6494,9 @@
       <c r="W105" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="X105" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="7" t="n">
@@ -6277,6 +6560,9 @@
       </c>
       <c r="V106" s="8" t="n"/>
       <c r="W106" s="8" t="n"/>
+      <c r="X106" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="7" t="n">
@@ -6328,6 +6614,9 @@
         <v>401408</v>
       </c>
       <c r="W107" s="8" t="n"/>
+      <c r="X107" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="7" t="n">
@@ -6377,6 +6666,9 @@
       <c r="W108" s="8" t="n">
         <v>200704</v>
       </c>
+      <c r="X108" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="7" t="n">
@@ -6426,6 +6718,7 @@
       <c r="U109" s="8" t="n"/>
       <c r="V109" s="8" t="n"/>
       <c r="W109" s="8" t="n"/>
+      <c r="X109" s="8" t="n"/>
     </row>
     <row r="110">
       <c r="A110" s="7" t="n">
@@ -6489,6 +6782,9 @@
       </c>
       <c r="V110" s="8" t="n"/>
       <c r="W110" s="8" t="n"/>
+      <c r="X110" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="7" t="n">
@@ -6540,6 +6836,9 @@
         <v>100352</v>
       </c>
       <c r="W111" s="8" t="n"/>
+      <c r="X111" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="7" t="n">
@@ -6589,6 +6888,9 @@
       <c r="W112" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="X112" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="7" t="n">
@@ -6652,6 +6954,9 @@
       </c>
       <c r="V113" s="8" t="n"/>
       <c r="W113" s="8" t="n"/>
+      <c r="X113" s="8" t="n">
+        <v>115605504</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="7" t="n">
@@ -6703,6 +7008,9 @@
         <v>100352</v>
       </c>
       <c r="W114" s="8" t="n"/>
+      <c r="X114" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="7" t="n">
@@ -6752,6 +7060,9 @@
       <c r="W115" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="X115" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="7" t="n">
@@ -6815,6 +7126,9 @@
       </c>
       <c r="V116" s="8" t="n"/>
       <c r="W116" s="8" t="n"/>
+      <c r="X116" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="7" t="n">
@@ -6866,6 +7180,9 @@
         <v>401408</v>
       </c>
       <c r="W117" s="8" t="n"/>
+      <c r="X117" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="7" t="n">
@@ -6915,6 +7232,9 @@
       <c r="W118" s="8" t="n">
         <v>200704</v>
       </c>
+      <c r="X118" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="7" t="n">
@@ -6964,6 +7284,7 @@
       <c r="U119" s="8" t="n"/>
       <c r="V119" s="8" t="n"/>
       <c r="W119" s="8" t="n"/>
+      <c r="X119" s="8" t="n"/>
     </row>
     <row r="120">
       <c r="A120" s="7" t="n">
@@ -7027,6 +7348,9 @@
       </c>
       <c r="V120" s="8" t="n"/>
       <c r="W120" s="8" t="n"/>
+      <c r="X120" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="7" t="n">
@@ -7078,6 +7402,9 @@
         <v>100352</v>
       </c>
       <c r="W121" s="8" t="n"/>
+      <c r="X121" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="7" t="n">
@@ -7127,6 +7454,9 @@
       <c r="W122" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="X122" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="7" t="n">
@@ -7190,6 +7520,9 @@
       </c>
       <c r="V123" s="8" t="n"/>
       <c r="W123" s="8" t="n"/>
+      <c r="X123" s="8" t="n">
+        <v>115605504</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="7" t="n">
@@ -7241,6 +7574,9 @@
         <v>100352</v>
       </c>
       <c r="W124" s="8" t="n"/>
+      <c r="X124" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="7" t="n">
@@ -7290,6 +7626,9 @@
       <c r="W125" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="X125" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="7" t="n">
@@ -7353,6 +7692,9 @@
       </c>
       <c r="V126" s="8" t="n"/>
       <c r="W126" s="8" t="n"/>
+      <c r="X126" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="7" t="n">
@@ -7404,6 +7746,9 @@
         <v>401408</v>
       </c>
       <c r="W127" s="8" t="n"/>
+      <c r="X127" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="7" t="n">
@@ -7453,6 +7798,9 @@
       <c r="W128" s="8" t="n">
         <v>200704</v>
       </c>
+      <c r="X128" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="7" t="n">
@@ -7502,6 +7850,7 @@
       <c r="U129" s="8" t="n"/>
       <c r="V129" s="8" t="n"/>
       <c r="W129" s="8" t="n"/>
+      <c r="X129" s="8" t="n"/>
     </row>
     <row r="130">
       <c r="A130" s="7" t="n">
@@ -7565,6 +7914,9 @@
       </c>
       <c r="V130" s="8" t="n"/>
       <c r="W130" s="8" t="n"/>
+      <c r="X130" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="7" t="n">
@@ -7616,6 +7968,9 @@
         <v>100352</v>
       </c>
       <c r="W131" s="8" t="n"/>
+      <c r="X131" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="7" t="n">
@@ -7665,6 +8020,9 @@
       <c r="W132" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="X132" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="7" t="n">
@@ -7728,6 +8086,9 @@
       </c>
       <c r="V133" s="8" t="n"/>
       <c r="W133" s="8" t="n"/>
+      <c r="X133" s="8" t="n">
+        <v>115605504</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="7" t="n">
@@ -7779,6 +8140,9 @@
         <v>100352</v>
       </c>
       <c r="W134" s="8" t="n"/>
+      <c r="X134" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="7" t="n">
@@ -7828,6 +8192,9 @@
       <c r="W135" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="X135" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="7" t="n">
@@ -7891,6 +8258,9 @@
       </c>
       <c r="V136" s="8" t="n"/>
       <c r="W136" s="8" t="n"/>
+      <c r="X136" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="7" t="n">
@@ -7942,6 +8312,9 @@
         <v>401408</v>
       </c>
       <c r="W137" s="8" t="n"/>
+      <c r="X137" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="7" t="n">
@@ -7991,6 +8364,9 @@
       <c r="W138" s="8" t="n">
         <v>200704</v>
       </c>
+      <c r="X138" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="7" t="n">
@@ -8040,6 +8416,7 @@
       <c r="U139" s="8" t="n"/>
       <c r="V139" s="8" t="n"/>
       <c r="W139" s="8" t="n"/>
+      <c r="X139" s="8" t="n"/>
     </row>
     <row r="140">
       <c r="A140" s="7" t="n">
@@ -8103,6 +8480,9 @@
       </c>
       <c r="V140" s="8" t="n"/>
       <c r="W140" s="8" t="n"/>
+      <c r="X140" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="7" t="n">
@@ -8154,6 +8534,9 @@
         <v>100352</v>
       </c>
       <c r="W141" s="8" t="n"/>
+      <c r="X141" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="7" t="n">
@@ -8203,6 +8586,9 @@
       <c r="W142" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="X142" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="7" t="n">
@@ -8266,6 +8652,9 @@
       </c>
       <c r="V143" s="8" t="n"/>
       <c r="W143" s="8" t="n"/>
+      <c r="X143" s="8" t="n">
+        <v>115605504</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="7" t="n">
@@ -8317,6 +8706,9 @@
         <v>100352</v>
       </c>
       <c r="W144" s="8" t="n"/>
+      <c r="X144" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="7" t="n">
@@ -8366,6 +8758,9 @@
       <c r="W145" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="X145" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="7" t="n">
@@ -8429,6 +8824,9 @@
       </c>
       <c r="V146" s="8" t="n"/>
       <c r="W146" s="8" t="n"/>
+      <c r="X146" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="7" t="n">
@@ -8480,6 +8878,9 @@
         <v>401408</v>
       </c>
       <c r="W147" s="8" t="n"/>
+      <c r="X147" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="7" t="n">
@@ -8529,6 +8930,9 @@
       <c r="W148" s="8" t="n">
         <v>200704</v>
       </c>
+      <c r="X148" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="7" t="n">
@@ -8576,6 +8980,7 @@
       <c r="U149" s="8" t="n"/>
       <c r="V149" s="8" t="n"/>
       <c r="W149" s="8" t="n"/>
+      <c r="X149" s="8" t="n"/>
     </row>
     <row r="150">
       <c r="A150" s="7" t="n">
@@ -8625,6 +9030,7 @@
       <c r="U150" s="8" t="n"/>
       <c r="V150" s="8" t="n"/>
       <c r="W150" s="8" t="n"/>
+      <c r="X150" s="8" t="n"/>
     </row>
     <row r="151">
       <c r="A151" s="7" t="n">
@@ -8688,6 +9094,9 @@
       </c>
       <c r="V151" s="8" t="n"/>
       <c r="W151" s="8" t="n"/>
+      <c r="X151" s="8" t="n">
+        <v>102760448</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="7" t="n">
@@ -8739,6 +9148,9 @@
         <v>200704</v>
       </c>
       <c r="W152" s="8" t="n"/>
+      <c r="X152" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="7" t="n">
@@ -8788,6 +9200,9 @@
       <c r="W153" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="X153" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="7" t="n">
@@ -8847,10 +9262,13 @@
         <v>2359296</v>
       </c>
       <c r="U154" s="8" t="n">
-        <v>115605504</v>
+        <v>462422016</v>
       </c>
       <c r="V154" s="8" t="n"/>
       <c r="W154" s="8" t="n"/>
+      <c r="X154" s="8" t="n">
+        <v>462422016</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="7" t="n">
@@ -8902,6 +9320,9 @@
         <v>50176</v>
       </c>
       <c r="W155" s="8" t="n"/>
+      <c r="X155" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="7" t="n">
@@ -8951,6 +9372,9 @@
       <c r="W156" s="8" t="n">
         <v>25088</v>
       </c>
+      <c r="X156" s="8" t="n">
+        <v>25088</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="7" t="n">
@@ -9014,6 +9438,9 @@
       </c>
       <c r="V157" s="8" t="n"/>
       <c r="W157" s="8" t="n"/>
+      <c r="X157" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="7" t="n">
@@ -9065,6 +9492,9 @@
         <v>200704</v>
       </c>
       <c r="W158" s="8" t="n"/>
+      <c r="X158" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="7" t="n">
@@ -9112,6 +9542,7 @@
       <c r="U159" s="8" t="n"/>
       <c r="V159" s="8" t="n"/>
       <c r="W159" s="8" t="n"/>
+      <c r="X159" s="8" t="n"/>
     </row>
     <row r="160">
       <c r="A160" s="7" t="n">
@@ -9171,10 +9602,13 @@
         <v>2097152</v>
       </c>
       <c r="U160" s="8" t="n">
-        <v>102760448</v>
+        <v>411041792</v>
       </c>
       <c r="V160" s="8" t="n"/>
       <c r="W160" s="8" t="n"/>
+      <c r="X160" s="8" t="n">
+        <v>411041792</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="7" t="n">
@@ -9226,6 +9660,9 @@
         <v>200704</v>
       </c>
       <c r="W161" s="8" t="n"/>
+      <c r="X161" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="7" t="n">
@@ -9275,6 +9712,9 @@
       <c r="W162" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="X162" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="7" t="n">
@@ -9324,6 +9764,7 @@
       <c r="U163" s="8" t="n"/>
       <c r="V163" s="8" t="n"/>
       <c r="W163" s="8" t="n"/>
+      <c r="X163" s="8" t="n"/>
     </row>
     <row r="164">
       <c r="A164" s="7" t="n">
@@ -9387,6 +9828,9 @@
       </c>
       <c r="V164" s="8" t="n"/>
       <c r="W164" s="8" t="n"/>
+      <c r="X164" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="7" t="n">
@@ -9438,6 +9882,9 @@
         <v>50176</v>
       </c>
       <c r="W165" s="8" t="n"/>
+      <c r="X165" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="7" t="n">
@@ -9487,6 +9934,9 @@
       <c r="W166" s="8" t="n">
         <v>25088</v>
       </c>
+      <c r="X166" s="8" t="n">
+        <v>25088</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="7" t="n">
@@ -9550,6 +10000,9 @@
       </c>
       <c r="V167" s="8" t="n"/>
       <c r="W167" s="8" t="n"/>
+      <c r="X167" s="8" t="n">
+        <v>115605504</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="7" t="n">
@@ -9601,6 +10054,9 @@
         <v>50176</v>
       </c>
       <c r="W168" s="8" t="n"/>
+      <c r="X168" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="7" t="n">
@@ -9650,6 +10106,9 @@
       <c r="W169" s="8" t="n">
         <v>25088</v>
       </c>
+      <c r="X169" s="8" t="n">
+        <v>25088</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="7" t="n">
@@ -9713,6 +10172,9 @@
       </c>
       <c r="V170" s="8" t="n"/>
       <c r="W170" s="8" t="n"/>
+      <c r="X170" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="7" t="n">
@@ -9764,6 +10226,9 @@
         <v>200704</v>
       </c>
       <c r="W171" s="8" t="n"/>
+      <c r="X171" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="7" t="n">
@@ -9813,6 +10278,9 @@
       <c r="W172" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="X172" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="7" t="n">
@@ -9862,6 +10330,7 @@
       <c r="U173" s="8" t="n"/>
       <c r="V173" s="8" t="n"/>
       <c r="W173" s="8" t="n"/>
+      <c r="X173" s="8" t="n"/>
     </row>
     <row r="174">
       <c r="A174" s="7" t="n">
@@ -9925,6 +10394,9 @@
       </c>
       <c r="V174" s="8" t="n"/>
       <c r="W174" s="8" t="n"/>
+      <c r="X174" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="7" t="n">
@@ -9976,6 +10448,9 @@
         <v>50176</v>
       </c>
       <c r="W175" s="8" t="n"/>
+      <c r="X175" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="7" t="n">
@@ -10025,6 +10500,9 @@
       <c r="W176" s="8" t="n">
         <v>25088</v>
       </c>
+      <c r="X176" s="8" t="n">
+        <v>25088</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="7" t="n">
@@ -10088,6 +10566,9 @@
       </c>
       <c r="V177" s="8" t="n"/>
       <c r="W177" s="8" t="n"/>
+      <c r="X177" s="8" t="n">
+        <v>115605504</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="7" t="n">
@@ -10139,6 +10620,9 @@
         <v>50176</v>
       </c>
       <c r="W178" s="8" t="n"/>
+      <c r="X178" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="7" t="n">
@@ -10188,6 +10672,9 @@
       <c r="W179" s="8" t="n">
         <v>25088</v>
       </c>
+      <c r="X179" s="8" t="n">
+        <v>25088</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="7" t="n">
@@ -10251,6 +10738,9 @@
       </c>
       <c r="V180" s="8" t="n"/>
       <c r="W180" s="8" t="n"/>
+      <c r="X180" s="8" t="n">
+        <v>51380224</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="7" t="n">
@@ -10302,6 +10792,9 @@
         <v>200704</v>
       </c>
       <c r="W181" s="8" t="n"/>
+      <c r="X181" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="7" t="n">
@@ -10351,6 +10844,9 @@
       <c r="W182" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="X182" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="7" t="n">
@@ -10398,6 +10894,7 @@
       <c r="U183" s="8" t="n"/>
       <c r="V183" s="8" t="n"/>
       <c r="W183" s="8" t="n"/>
+      <c r="X183" s="8" t="n"/>
     </row>
     <row r="184">
       <c r="A184" s="7" t="n">
@@ -10441,6 +10938,9 @@
       </c>
       <c r="V184" s="8" t="n"/>
       <c r="W184" s="8" t="n"/>
+      <c r="X184" s="8" t="n">
+        <v>2048000</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -10451,7 +10951,7 @@
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:T1"/>
-    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="U1:X1"/>
   </mergeCells>
   <conditionalFormatting sqref="S1:S184">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
@@ -10465,7 +10965,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U184">
     <cfRule type="cellIs" priority="3" operator="equal" dxfId="2" stopIfTrue="1">
-      <formula>118013952</formula>
+      <formula>472055808</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10524,7 +11024,7 @@
         </is>
       </c>
       <c r="B4" s="8" t="n">
-        <v>4.089184256</v>
+        <v>6.40851968</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve backprop by splitting columns for more details
</commit_message>
<xml_diff>
--- a/outputs/torch/resnet50.xlsx
+++ b/outputs/torch/resnet50.xlsx
@@ -123,7 +123,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -142,6 +142,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="0000FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="00FFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -507,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X184"/>
+  <dimension ref="A1:Z184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -571,12 +578,18 @@
       <c r="T1" s="12" t="n"/>
       <c r="U1" s="10" t="inlineStr">
         <is>
-          <t>Operation Summary</t>
+          <t>Forward Ops</t>
         </is>
       </c>
       <c r="V1" s="11" t="n"/>
-      <c r="W1" s="11" t="n"/>
-      <c r="X1" s="12" t="n"/>
+      <c r="W1" s="12" t="n"/>
+      <c r="X1" s="10" t="inlineStr">
+        <is>
+          <t>Backward Ops</t>
+        </is>
+      </c>
+      <c r="Y1" s="11" t="n"/>
+      <c r="Z1" s="12" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="10" t="inlineStr"/>
@@ -692,7 +705,17 @@
       </c>
       <c r="X2" s="10" t="inlineStr">
         <is>
-          <t>BackProp</t>
+          <t>GEMM</t>
+        </is>
+      </c>
+      <c r="Y2" s="10" t="inlineStr">
+        <is>
+          <t>ElemWise</t>
+        </is>
+      </c>
+      <c r="Z2" s="10" t="inlineStr">
+        <is>
+          <t>Activation</t>
         </is>
       </c>
     </row>
@@ -754,13 +777,15 @@
         <v>9408</v>
       </c>
       <c r="U3" s="8" t="n">
-        <v>472055808</v>
+        <v>118013952</v>
       </c>
       <c r="V3" s="8" t="n"/>
       <c r="W3" s="8" t="n"/>
       <c r="X3" s="8" t="n">
         <v>472055808</v>
       </c>
+      <c r="Y3" s="8" t="n"/>
+      <c r="Z3" s="8" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="7" t="n">
@@ -812,9 +837,11 @@
         <v>1605632</v>
       </c>
       <c r="W4" s="8" t="n"/>
-      <c r="X4" s="8" t="n">
+      <c r="X4" s="8" t="n"/>
+      <c r="Y4" s="8" t="n">
         <v>1605632</v>
       </c>
+      <c r="Z4" s="8" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="7" t="n">
@@ -864,7 +891,9 @@
       <c r="W5" s="8" t="n">
         <v>802816</v>
       </c>
-      <c r="X5" s="8" t="n">
+      <c r="X5" s="8" t="n"/>
+      <c r="Y5" s="8" t="n"/>
+      <c r="Z5" s="8" t="n">
         <v>802816</v>
       </c>
     </row>
@@ -924,9 +953,11 @@
         <v>1605632</v>
       </c>
       <c r="W6" s="8" t="n"/>
-      <c r="X6" s="8" t="n">
+      <c r="X6" s="8" t="n"/>
+      <c r="Y6" s="8" t="n">
         <v>2517630976</v>
       </c>
+      <c r="Z6" s="8" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="7" t="n">
@@ -975,6 +1006,8 @@
       <c r="V7" s="8" t="n"/>
       <c r="W7" s="8" t="n"/>
       <c r="X7" s="8" t="n"/>
+      <c r="Y7" s="8" t="n"/>
+      <c r="Z7" s="8" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="7" t="n">
@@ -1025,6 +1058,8 @@
       <c r="V8" s="8" t="n"/>
       <c r="W8" s="8" t="n"/>
       <c r="X8" s="8" t="n"/>
+      <c r="Y8" s="8" t="n"/>
+      <c r="Z8" s="8" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="7" t="n">
@@ -1091,6 +1126,8 @@
       <c r="X9" s="8" t="n">
         <v>12845056</v>
       </c>
+      <c r="Y9" s="8" t="n"/>
+      <c r="Z9" s="8" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="7" t="n">
@@ -1142,9 +1179,11 @@
         <v>401408</v>
       </c>
       <c r="W10" s="8" t="n"/>
-      <c r="X10" s="8" t="n">
+      <c r="X10" s="8" t="n"/>
+      <c r="Y10" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="Z10" s="8" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="7" t="n">
@@ -1194,7 +1233,9 @@
       <c r="W11" s="8" t="n">
         <v>200704</v>
       </c>
-      <c r="X11" s="8" t="n">
+      <c r="X11" s="8" t="n"/>
+      <c r="Y11" s="8" t="n"/>
+      <c r="Z11" s="8" t="n">
         <v>200704</v>
       </c>
     </row>
@@ -1263,6 +1304,8 @@
       <c r="X12" s="8" t="n">
         <v>115605504</v>
       </c>
+      <c r="Y12" s="8" t="n"/>
+      <c r="Z12" s="8" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="7" t="n">
@@ -1314,9 +1357,11 @@
         <v>401408</v>
       </c>
       <c r="W13" s="8" t="n"/>
-      <c r="X13" s="8" t="n">
+      <c r="X13" s="8" t="n"/>
+      <c r="Y13" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="Z13" s="8" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="7" t="n">
@@ -1366,7 +1411,9 @@
       <c r="W14" s="8" t="n">
         <v>200704</v>
       </c>
-      <c r="X14" s="8" t="n">
+      <c r="X14" s="8" t="n"/>
+      <c r="Y14" s="8" t="n"/>
+      <c r="Z14" s="8" t="n">
         <v>200704</v>
       </c>
     </row>
@@ -1435,6 +1482,8 @@
       <c r="X15" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y15" s="8" t="n"/>
+      <c r="Z15" s="8" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="7" t="n">
@@ -1486,9 +1535,11 @@
         <v>1605632</v>
       </c>
       <c r="W16" s="8" t="n"/>
-      <c r="X16" s="8" t="n">
+      <c r="X16" s="8" t="n"/>
+      <c r="Y16" s="8" t="n">
         <v>1605632</v>
       </c>
+      <c r="Z16" s="8" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="7" t="n">
@@ -1537,6 +1588,8 @@
       <c r="V17" s="8" t="n"/>
       <c r="W17" s="8" t="n"/>
       <c r="X17" s="8" t="n"/>
+      <c r="Y17" s="8" t="n"/>
+      <c r="Z17" s="8" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="7" t="n">
@@ -1603,6 +1656,8 @@
       <c r="X18" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y18" s="8" t="n"/>
+      <c r="Z18" s="8" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="7" t="n">
@@ -1654,9 +1709,11 @@
         <v>1605632</v>
       </c>
       <c r="W19" s="8" t="n"/>
-      <c r="X19" s="8" t="n">
+      <c r="X19" s="8" t="n"/>
+      <c r="Y19" s="8" t="n">
         <v>1605632</v>
       </c>
+      <c r="Z19" s="8" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="7" t="n">
@@ -1706,7 +1763,9 @@
       <c r="W20" s="8" t="n">
         <v>802816</v>
       </c>
-      <c r="X20" s="8" t="n">
+      <c r="X20" s="8" t="n"/>
+      <c r="Y20" s="8" t="n"/>
+      <c r="Z20" s="8" t="n">
         <v>802816</v>
       </c>
     </row>
@@ -1759,6 +1818,8 @@
       <c r="V21" s="8" t="n"/>
       <c r="W21" s="8" t="n"/>
       <c r="X21" s="8" t="n"/>
+      <c r="Y21" s="8" t="n"/>
+      <c r="Z21" s="8" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="7" t="n">
@@ -1825,6 +1886,8 @@
       <c r="X22" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y22" s="8" t="n"/>
+      <c r="Z22" s="8" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="7" t="n">
@@ -1876,9 +1939,11 @@
         <v>401408</v>
       </c>
       <c r="W23" s="8" t="n"/>
-      <c r="X23" s="8" t="n">
+      <c r="X23" s="8" t="n"/>
+      <c r="Y23" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="Z23" s="8" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="7" t="n">
@@ -1928,7 +1993,9 @@
       <c r="W24" s="8" t="n">
         <v>200704</v>
       </c>
-      <c r="X24" s="8" t="n">
+      <c r="X24" s="8" t="n"/>
+      <c r="Y24" s="8" t="n"/>
+      <c r="Z24" s="8" t="n">
         <v>200704</v>
       </c>
     </row>
@@ -1997,6 +2064,8 @@
       <c r="X25" s="8" t="n">
         <v>115605504</v>
       </c>
+      <c r="Y25" s="8" t="n"/>
+      <c r="Z25" s="8" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="7" t="n">
@@ -2048,9 +2117,11 @@
         <v>401408</v>
       </c>
       <c r="W26" s="8" t="n"/>
-      <c r="X26" s="8" t="n">
+      <c r="X26" s="8" t="n"/>
+      <c r="Y26" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="Z26" s="8" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="7" t="n">
@@ -2100,7 +2171,9 @@
       <c r="W27" s="8" t="n">
         <v>200704</v>
       </c>
-      <c r="X27" s="8" t="n">
+      <c r="X27" s="8" t="n"/>
+      <c r="Y27" s="8" t="n"/>
+      <c r="Z27" s="8" t="n">
         <v>200704</v>
       </c>
     </row>
@@ -2169,6 +2242,8 @@
       <c r="X28" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y28" s="8" t="n"/>
+      <c r="Z28" s="8" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="7" t="n">
@@ -2220,9 +2295,11 @@
         <v>1605632</v>
       </c>
       <c r="W29" s="8" t="n"/>
-      <c r="X29" s="8" t="n">
+      <c r="X29" s="8" t="n"/>
+      <c r="Y29" s="8" t="n">
         <v>1605632</v>
       </c>
+      <c r="Z29" s="8" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="7" t="n">
@@ -2272,7 +2349,9 @@
       <c r="W30" s="8" t="n">
         <v>802816</v>
       </c>
-      <c r="X30" s="8" t="n">
+      <c r="X30" s="8" t="n"/>
+      <c r="Y30" s="8" t="n"/>
+      <c r="Z30" s="8" t="n">
         <v>802816</v>
       </c>
     </row>
@@ -2325,6 +2404,8 @@
       <c r="V31" s="8" t="n"/>
       <c r="W31" s="8" t="n"/>
       <c r="X31" s="8" t="n"/>
+      <c r="Y31" s="8" t="n"/>
+      <c r="Z31" s="8" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="7" t="n">
@@ -2391,6 +2472,8 @@
       <c r="X32" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y32" s="8" t="n"/>
+      <c r="Z32" s="8" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="7" t="n">
@@ -2442,9 +2525,11 @@
         <v>401408</v>
       </c>
       <c r="W33" s="8" t="n"/>
-      <c r="X33" s="8" t="n">
+      <c r="X33" s="8" t="n"/>
+      <c r="Y33" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="Z33" s="8" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="7" t="n">
@@ -2494,7 +2579,9 @@
       <c r="W34" s="8" t="n">
         <v>200704</v>
       </c>
-      <c r="X34" s="8" t="n">
+      <c r="X34" s="8" t="n"/>
+      <c r="Y34" s="8" t="n"/>
+      <c r="Z34" s="8" t="n">
         <v>200704</v>
       </c>
     </row>
@@ -2563,6 +2650,8 @@
       <c r="X35" s="8" t="n">
         <v>115605504</v>
       </c>
+      <c r="Y35" s="8" t="n"/>
+      <c r="Z35" s="8" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="7" t="n">
@@ -2614,9 +2703,11 @@
         <v>401408</v>
       </c>
       <c r="W36" s="8" t="n"/>
-      <c r="X36" s="8" t="n">
+      <c r="X36" s="8" t="n"/>
+      <c r="Y36" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="Z36" s="8" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="7" t="n">
@@ -2666,7 +2757,9 @@
       <c r="W37" s="8" t="n">
         <v>200704</v>
       </c>
-      <c r="X37" s="8" t="n">
+      <c r="X37" s="8" t="n"/>
+      <c r="Y37" s="8" t="n"/>
+      <c r="Z37" s="8" t="n">
         <v>200704</v>
       </c>
     </row>
@@ -2735,6 +2828,8 @@
       <c r="X38" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y38" s="8" t="n"/>
+      <c r="Z38" s="8" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="7" t="n">
@@ -2786,9 +2881,11 @@
         <v>1605632</v>
       </c>
       <c r="W39" s="8" t="n"/>
-      <c r="X39" s="8" t="n">
+      <c r="X39" s="8" t="n"/>
+      <c r="Y39" s="8" t="n">
         <v>1605632</v>
       </c>
+      <c r="Z39" s="8" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="7" t="n">
@@ -2838,7 +2935,9 @@
       <c r="W40" s="8" t="n">
         <v>802816</v>
       </c>
-      <c r="X40" s="8" t="n">
+      <c r="X40" s="8" t="n"/>
+      <c r="Y40" s="8" t="n"/>
+      <c r="Z40" s="8" t="n">
         <v>802816</v>
       </c>
     </row>
@@ -2889,6 +2988,8 @@
       <c r="V41" s="8" t="n"/>
       <c r="W41" s="8" t="n"/>
       <c r="X41" s="8" t="n"/>
+      <c r="Y41" s="8" t="n"/>
+      <c r="Z41" s="8" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="7" t="n">
@@ -2939,6 +3040,8 @@
       <c r="V42" s="8" t="n"/>
       <c r="W42" s="8" t="n"/>
       <c r="X42" s="8" t="n"/>
+      <c r="Y42" s="8" t="n"/>
+      <c r="Z42" s="8" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="7" t="n">
@@ -3005,6 +3108,8 @@
       <c r="X43" s="8" t="n">
         <v>102760448</v>
       </c>
+      <c r="Y43" s="8" t="n"/>
+      <c r="Z43" s="8" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="7" t="n">
@@ -3056,9 +3161,11 @@
         <v>802816</v>
       </c>
       <c r="W44" s="8" t="n"/>
-      <c r="X44" s="8" t="n">
+      <c r="X44" s="8" t="n"/>
+      <c r="Y44" s="8" t="n">
         <v>802816</v>
       </c>
+      <c r="Z44" s="8" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="7" t="n">
@@ -3108,7 +3215,9 @@
       <c r="W45" s="8" t="n">
         <v>401408</v>
       </c>
-      <c r="X45" s="8" t="n">
+      <c r="X45" s="8" t="n"/>
+      <c r="Y45" s="8" t="n"/>
+      <c r="Z45" s="8" t="n">
         <v>401408</v>
       </c>
     </row>
@@ -3170,13 +3279,15 @@
         <v>147456</v>
       </c>
       <c r="U46" s="8" t="n">
-        <v>462422016</v>
+        <v>115605504</v>
       </c>
       <c r="V46" s="8" t="n"/>
       <c r="W46" s="8" t="n"/>
       <c r="X46" s="8" t="n">
         <v>462422016</v>
       </c>
+      <c r="Y46" s="8" t="n"/>
+      <c r="Z46" s="8" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="7" t="n">
@@ -3228,9 +3339,11 @@
         <v>200704</v>
       </c>
       <c r="W47" s="8" t="n"/>
-      <c r="X47" s="8" t="n">
-        <v>200704</v>
-      </c>
+      <c r="X47" s="8" t="n"/>
+      <c r="Y47" s="8" t="n">
+        <v>200704</v>
+      </c>
+      <c r="Z47" s="8" t="n"/>
     </row>
     <row r="48">
       <c r="A48" s="7" t="n">
@@ -3280,7 +3393,9 @@
       <c r="W48" s="8" t="n">
         <v>100352</v>
       </c>
-      <c r="X48" s="8" t="n">
+      <c r="X48" s="8" t="n"/>
+      <c r="Y48" s="8" t="n"/>
+      <c r="Z48" s="8" t="n">
         <v>100352</v>
       </c>
     </row>
@@ -3349,6 +3464,8 @@
       <c r="X49" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y49" s="8" t="n"/>
+      <c r="Z49" s="8" t="n"/>
     </row>
     <row r="50">
       <c r="A50" s="7" t="n">
@@ -3400,9 +3517,11 @@
         <v>802816</v>
       </c>
       <c r="W50" s="8" t="n"/>
-      <c r="X50" s="8" t="n">
+      <c r="X50" s="8" t="n"/>
+      <c r="Y50" s="8" t="n">
         <v>802816</v>
       </c>
+      <c r="Z50" s="8" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="7" t="n">
@@ -3451,6 +3570,8 @@
       <c r="V51" s="8" t="n"/>
       <c r="W51" s="8" t="n"/>
       <c r="X51" s="8" t="n"/>
+      <c r="Y51" s="8" t="n"/>
+      <c r="Z51" s="8" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="7" t="n">
@@ -3510,13 +3631,15 @@
         <v>131072</v>
       </c>
       <c r="U52" s="8" t="n">
-        <v>411041792</v>
+        <v>102760448</v>
       </c>
       <c r="V52" s="8" t="n"/>
       <c r="W52" s="8" t="n"/>
       <c r="X52" s="8" t="n">
         <v>411041792</v>
       </c>
+      <c r="Y52" s="8" t="n"/>
+      <c r="Z52" s="8" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="7" t="n">
@@ -3568,9 +3691,11 @@
         <v>802816</v>
       </c>
       <c r="W53" s="8" t="n"/>
-      <c r="X53" s="8" t="n">
+      <c r="X53" s="8" t="n"/>
+      <c r="Y53" s="8" t="n">
         <v>802816</v>
       </c>
+      <c r="Z53" s="8" t="n"/>
     </row>
     <row r="54">
       <c r="A54" s="7" t="n">
@@ -3620,7 +3745,9 @@
       <c r="W54" s="8" t="n">
         <v>401408</v>
       </c>
-      <c r="X54" s="8" t="n">
+      <c r="X54" s="8" t="n"/>
+      <c r="Y54" s="8" t="n"/>
+      <c r="Z54" s="8" t="n">
         <v>401408</v>
       </c>
     </row>
@@ -3673,6 +3800,8 @@
       <c r="V55" s="8" t="n"/>
       <c r="W55" s="8" t="n"/>
       <c r="X55" s="8" t="n"/>
+      <c r="Y55" s="8" t="n"/>
+      <c r="Z55" s="8" t="n"/>
     </row>
     <row r="56">
       <c r="A56" s="7" t="n">
@@ -3739,6 +3868,8 @@
       <c r="X56" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y56" s="8" t="n"/>
+      <c r="Z56" s="8" t="n"/>
     </row>
     <row r="57">
       <c r="A57" s="7" t="n">
@@ -3790,9 +3921,11 @@
         <v>200704</v>
       </c>
       <c r="W57" s="8" t="n"/>
-      <c r="X57" s="8" t="n">
-        <v>200704</v>
-      </c>
+      <c r="X57" s="8" t="n"/>
+      <c r="Y57" s="8" t="n">
+        <v>200704</v>
+      </c>
+      <c r="Z57" s="8" t="n"/>
     </row>
     <row r="58">
       <c r="A58" s="7" t="n">
@@ -3842,7 +3975,9 @@
       <c r="W58" s="8" t="n">
         <v>100352</v>
       </c>
-      <c r="X58" s="8" t="n">
+      <c r="X58" s="8" t="n"/>
+      <c r="Y58" s="8" t="n"/>
+      <c r="Z58" s="8" t="n">
         <v>100352</v>
       </c>
     </row>
@@ -3911,6 +4046,8 @@
       <c r="X59" s="8" t="n">
         <v>115605504</v>
       </c>
+      <c r="Y59" s="8" t="n"/>
+      <c r="Z59" s="8" t="n"/>
     </row>
     <row r="60">
       <c r="A60" s="7" t="n">
@@ -3962,9 +4099,11 @@
         <v>200704</v>
       </c>
       <c r="W60" s="8" t="n"/>
-      <c r="X60" s="8" t="n">
-        <v>200704</v>
-      </c>
+      <c r="X60" s="8" t="n"/>
+      <c r="Y60" s="8" t="n">
+        <v>200704</v>
+      </c>
+      <c r="Z60" s="8" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="7" t="n">
@@ -4014,7 +4153,9 @@
       <c r="W61" s="8" t="n">
         <v>100352</v>
       </c>
-      <c r="X61" s="8" t="n">
+      <c r="X61" s="8" t="n"/>
+      <c r="Y61" s="8" t="n"/>
+      <c r="Z61" s="8" t="n">
         <v>100352</v>
       </c>
     </row>
@@ -4083,6 +4224,8 @@
       <c r="X62" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y62" s="8" t="n"/>
+      <c r="Z62" s="8" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="7" t="n">
@@ -4134,9 +4277,11 @@
         <v>802816</v>
       </c>
       <c r="W63" s="8" t="n"/>
-      <c r="X63" s="8" t="n">
+      <c r="X63" s="8" t="n"/>
+      <c r="Y63" s="8" t="n">
         <v>802816</v>
       </c>
+      <c r="Z63" s="8" t="n"/>
     </row>
     <row r="64">
       <c r="A64" s="7" t="n">
@@ -4186,7 +4331,9 @@
       <c r="W64" s="8" t="n">
         <v>401408</v>
       </c>
-      <c r="X64" s="8" t="n">
+      <c r="X64" s="8" t="n"/>
+      <c r="Y64" s="8" t="n"/>
+      <c r="Z64" s="8" t="n">
         <v>401408</v>
       </c>
     </row>
@@ -4239,6 +4386,8 @@
       <c r="V65" s="8" t="n"/>
       <c r="W65" s="8" t="n"/>
       <c r="X65" s="8" t="n"/>
+      <c r="Y65" s="8" t="n"/>
+      <c r="Z65" s="8" t="n"/>
     </row>
     <row r="66">
       <c r="A66" s="7" t="n">
@@ -4305,6 +4454,8 @@
       <c r="X66" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y66" s="8" t="n"/>
+      <c r="Z66" s="8" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="7" t="n">
@@ -4356,9 +4507,11 @@
         <v>200704</v>
       </c>
       <c r="W67" s="8" t="n"/>
-      <c r="X67" s="8" t="n">
-        <v>200704</v>
-      </c>
+      <c r="X67" s="8" t="n"/>
+      <c r="Y67" s="8" t="n">
+        <v>200704</v>
+      </c>
+      <c r="Z67" s="8" t="n"/>
     </row>
     <row r="68">
       <c r="A68" s="7" t="n">
@@ -4408,7 +4561,9 @@
       <c r="W68" s="8" t="n">
         <v>100352</v>
       </c>
-      <c r="X68" s="8" t="n">
+      <c r="X68" s="8" t="n"/>
+      <c r="Y68" s="8" t="n"/>
+      <c r="Z68" s="8" t="n">
         <v>100352</v>
       </c>
     </row>
@@ -4477,6 +4632,8 @@
       <c r="X69" s="8" t="n">
         <v>115605504</v>
       </c>
+      <c r="Y69" s="8" t="n"/>
+      <c r="Z69" s="8" t="n"/>
     </row>
     <row r="70">
       <c r="A70" s="7" t="n">
@@ -4528,9 +4685,11 @@
         <v>200704</v>
       </c>
       <c r="W70" s="8" t="n"/>
-      <c r="X70" s="8" t="n">
-        <v>200704</v>
-      </c>
+      <c r="X70" s="8" t="n"/>
+      <c r="Y70" s="8" t="n">
+        <v>200704</v>
+      </c>
+      <c r="Z70" s="8" t="n"/>
     </row>
     <row r="71">
       <c r="A71" s="7" t="n">
@@ -4580,7 +4739,9 @@
       <c r="W71" s="8" t="n">
         <v>100352</v>
       </c>
-      <c r="X71" s="8" t="n">
+      <c r="X71" s="8" t="n"/>
+      <c r="Y71" s="8" t="n"/>
+      <c r="Z71" s="8" t="n">
         <v>100352</v>
       </c>
     </row>
@@ -4649,6 +4810,8 @@
       <c r="X72" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y72" s="8" t="n"/>
+      <c r="Z72" s="8" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="7" t="n">
@@ -4700,9 +4863,11 @@
         <v>802816</v>
       </c>
       <c r="W73" s="8" t="n"/>
-      <c r="X73" s="8" t="n">
+      <c r="X73" s="8" t="n"/>
+      <c r="Y73" s="8" t="n">
         <v>802816</v>
       </c>
+      <c r="Z73" s="8" t="n"/>
     </row>
     <row r="74">
       <c r="A74" s="7" t="n">
@@ -4752,7 +4917,9 @@
       <c r="W74" s="8" t="n">
         <v>401408</v>
       </c>
-      <c r="X74" s="8" t="n">
+      <c r="X74" s="8" t="n"/>
+      <c r="Y74" s="8" t="n"/>
+      <c r="Z74" s="8" t="n">
         <v>401408</v>
       </c>
     </row>
@@ -4805,6 +4972,8 @@
       <c r="V75" s="8" t="n"/>
       <c r="W75" s="8" t="n"/>
       <c r="X75" s="8" t="n"/>
+      <c r="Y75" s="8" t="n"/>
+      <c r="Z75" s="8" t="n"/>
     </row>
     <row r="76">
       <c r="A76" s="7" t="n">
@@ -4871,6 +5040,8 @@
       <c r="X76" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y76" s="8" t="n"/>
+      <c r="Z76" s="8" t="n"/>
     </row>
     <row r="77">
       <c r="A77" s="7" t="n">
@@ -4922,9 +5093,11 @@
         <v>200704</v>
       </c>
       <c r="W77" s="8" t="n"/>
-      <c r="X77" s="8" t="n">
-        <v>200704</v>
-      </c>
+      <c r="X77" s="8" t="n"/>
+      <c r="Y77" s="8" t="n">
+        <v>200704</v>
+      </c>
+      <c r="Z77" s="8" t="n"/>
     </row>
     <row r="78">
       <c r="A78" s="7" t="n">
@@ -4974,7 +5147,9 @@
       <c r="W78" s="8" t="n">
         <v>100352</v>
       </c>
-      <c r="X78" s="8" t="n">
+      <c r="X78" s="8" t="n"/>
+      <c r="Y78" s="8" t="n"/>
+      <c r="Z78" s="8" t="n">
         <v>100352</v>
       </c>
     </row>
@@ -5043,6 +5218,8 @@
       <c r="X79" s="8" t="n">
         <v>115605504</v>
       </c>
+      <c r="Y79" s="8" t="n"/>
+      <c r="Z79" s="8" t="n"/>
     </row>
     <row r="80">
       <c r="A80" s="7" t="n">
@@ -5094,9 +5271,11 @@
         <v>200704</v>
       </c>
       <c r="W80" s="8" t="n"/>
-      <c r="X80" s="8" t="n">
-        <v>200704</v>
-      </c>
+      <c r="X80" s="8" t="n"/>
+      <c r="Y80" s="8" t="n">
+        <v>200704</v>
+      </c>
+      <c r="Z80" s="8" t="n"/>
     </row>
     <row r="81">
       <c r="A81" s="7" t="n">
@@ -5146,7 +5325,9 @@
       <c r="W81" s="8" t="n">
         <v>100352</v>
       </c>
-      <c r="X81" s="8" t="n">
+      <c r="X81" s="8" t="n"/>
+      <c r="Y81" s="8" t="n"/>
+      <c r="Z81" s="8" t="n">
         <v>100352</v>
       </c>
     </row>
@@ -5215,6 +5396,8 @@
       <c r="X82" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y82" s="8" t="n"/>
+      <c r="Z82" s="8" t="n"/>
     </row>
     <row r="83">
       <c r="A83" s="7" t="n">
@@ -5266,9 +5449,11 @@
         <v>802816</v>
       </c>
       <c r="W83" s="8" t="n"/>
-      <c r="X83" s="8" t="n">
+      <c r="X83" s="8" t="n"/>
+      <c r="Y83" s="8" t="n">
         <v>802816</v>
       </c>
+      <c r="Z83" s="8" t="n"/>
     </row>
     <row r="84">
       <c r="A84" s="7" t="n">
@@ -5318,7 +5503,9 @@
       <c r="W84" s="8" t="n">
         <v>401408</v>
       </c>
-      <c r="X84" s="8" t="n">
+      <c r="X84" s="8" t="n"/>
+      <c r="Y84" s="8" t="n"/>
+      <c r="Z84" s="8" t="n">
         <v>401408</v>
       </c>
     </row>
@@ -5369,6 +5556,8 @@
       <c r="V85" s="8" t="n"/>
       <c r="W85" s="8" t="n"/>
       <c r="X85" s="8" t="n"/>
+      <c r="Y85" s="8" t="n"/>
+      <c r="Z85" s="8" t="n"/>
     </row>
     <row r="86">
       <c r="A86" s="7" t="n">
@@ -5419,6 +5608,8 @@
       <c r="V86" s="8" t="n"/>
       <c r="W86" s="8" t="n"/>
       <c r="X86" s="8" t="n"/>
+      <c r="Y86" s="8" t="n"/>
+      <c r="Z86" s="8" t="n"/>
     </row>
     <row r="87">
       <c r="A87" s="7" t="n">
@@ -5485,6 +5676,8 @@
       <c r="X87" s="8" t="n">
         <v>102760448</v>
       </c>
+      <c r="Y87" s="8" t="n"/>
+      <c r="Z87" s="8" t="n"/>
     </row>
     <row r="88">
       <c r="A88" s="7" t="n">
@@ -5536,9 +5729,11 @@
         <v>401408</v>
       </c>
       <c r="W88" s="8" t="n"/>
-      <c r="X88" s="8" t="n">
+      <c r="X88" s="8" t="n"/>
+      <c r="Y88" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="Z88" s="8" t="n"/>
     </row>
     <row r="89">
       <c r="A89" s="7" t="n">
@@ -5588,7 +5783,9 @@
       <c r="W89" s="8" t="n">
         <v>200704</v>
       </c>
-      <c r="X89" s="8" t="n">
+      <c r="X89" s="8" t="n"/>
+      <c r="Y89" s="8" t="n"/>
+      <c r="Z89" s="8" t="n">
         <v>200704</v>
       </c>
     </row>
@@ -5650,13 +5847,15 @@
         <v>589824</v>
       </c>
       <c r="U90" s="8" t="n">
-        <v>462422016</v>
+        <v>115605504</v>
       </c>
       <c r="V90" s="8" t="n"/>
       <c r="W90" s="8" t="n"/>
       <c r="X90" s="8" t="n">
         <v>462422016</v>
       </c>
+      <c r="Y90" s="8" t="n"/>
+      <c r="Z90" s="8" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="7" t="n">
@@ -5708,9 +5907,11 @@
         <v>100352</v>
       </c>
       <c r="W91" s="8" t="n"/>
-      <c r="X91" s="8" t="n">
+      <c r="X91" s="8" t="n"/>
+      <c r="Y91" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="Z91" s="8" t="n"/>
     </row>
     <row r="92">
       <c r="A92" s="7" t="n">
@@ -5760,7 +5961,9 @@
       <c r="W92" s="8" t="n">
         <v>50176</v>
       </c>
-      <c r="X92" s="8" t="n">
+      <c r="X92" s="8" t="n"/>
+      <c r="Y92" s="8" t="n"/>
+      <c r="Z92" s="8" t="n">
         <v>50176</v>
       </c>
     </row>
@@ -5829,6 +6032,8 @@
       <c r="X93" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y93" s="8" t="n"/>
+      <c r="Z93" s="8" t="n"/>
     </row>
     <row r="94">
       <c r="A94" s="7" t="n">
@@ -5880,9 +6085,11 @@
         <v>401408</v>
       </c>
       <c r="W94" s="8" t="n"/>
-      <c r="X94" s="8" t="n">
+      <c r="X94" s="8" t="n"/>
+      <c r="Y94" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="Z94" s="8" t="n"/>
     </row>
     <row r="95">
       <c r="A95" s="7" t="n">
@@ -5931,6 +6138,8 @@
       <c r="V95" s="8" t="n"/>
       <c r="W95" s="8" t="n"/>
       <c r="X95" s="8" t="n"/>
+      <c r="Y95" s="8" t="n"/>
+      <c r="Z95" s="8" t="n"/>
     </row>
     <row r="96">
       <c r="A96" s="7" t="n">
@@ -5990,13 +6199,15 @@
         <v>524288</v>
       </c>
       <c r="U96" s="8" t="n">
-        <v>411041792</v>
+        <v>102760448</v>
       </c>
       <c r="V96" s="8" t="n"/>
       <c r="W96" s="8" t="n"/>
       <c r="X96" s="8" t="n">
         <v>411041792</v>
       </c>
+      <c r="Y96" s="8" t="n"/>
+      <c r="Z96" s="8" t="n"/>
     </row>
     <row r="97">
       <c r="A97" s="7" t="n">
@@ -6048,9 +6259,11 @@
         <v>401408</v>
       </c>
       <c r="W97" s="8" t="n"/>
-      <c r="X97" s="8" t="n">
+      <c r="X97" s="8" t="n"/>
+      <c r="Y97" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="Z97" s="8" t="n"/>
     </row>
     <row r="98">
       <c r="A98" s="7" t="n">
@@ -6100,7 +6313,9 @@
       <c r="W98" s="8" t="n">
         <v>200704</v>
       </c>
-      <c r="X98" s="8" t="n">
+      <c r="X98" s="8" t="n"/>
+      <c r="Y98" s="8" t="n"/>
+      <c r="Z98" s="8" t="n">
         <v>200704</v>
       </c>
     </row>
@@ -6153,6 +6368,8 @@
       <c r="V99" s="8" t="n"/>
       <c r="W99" s="8" t="n"/>
       <c r="X99" s="8" t="n"/>
+      <c r="Y99" s="8" t="n"/>
+      <c r="Z99" s="8" t="n"/>
     </row>
     <row r="100">
       <c r="A100" s="7" t="n">
@@ -6219,6 +6436,8 @@
       <c r="X100" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y100" s="8" t="n"/>
+      <c r="Z100" s="8" t="n"/>
     </row>
     <row r="101">
       <c r="A101" s="7" t="n">
@@ -6270,9 +6489,11 @@
         <v>100352</v>
       </c>
       <c r="W101" s="8" t="n"/>
-      <c r="X101" s="8" t="n">
+      <c r="X101" s="8" t="n"/>
+      <c r="Y101" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="Z101" s="8" t="n"/>
     </row>
     <row r="102">
       <c r="A102" s="7" t="n">
@@ -6322,7 +6543,9 @@
       <c r="W102" s="8" t="n">
         <v>50176</v>
       </c>
-      <c r="X102" s="8" t="n">
+      <c r="X102" s="8" t="n"/>
+      <c r="Y102" s="8" t="n"/>
+      <c r="Z102" s="8" t="n">
         <v>50176</v>
       </c>
     </row>
@@ -6391,6 +6614,8 @@
       <c r="X103" s="8" t="n">
         <v>115605504</v>
       </c>
+      <c r="Y103" s="8" t="n"/>
+      <c r="Z103" s="8" t="n"/>
     </row>
     <row r="104">
       <c r="A104" s="7" t="n">
@@ -6442,9 +6667,11 @@
         <v>100352</v>
       </c>
       <c r="W104" s="8" t="n"/>
-      <c r="X104" s="8" t="n">
+      <c r="X104" s="8" t="n"/>
+      <c r="Y104" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="Z104" s="8" t="n"/>
     </row>
     <row r="105">
       <c r="A105" s="7" t="n">
@@ -6494,7 +6721,9 @@
       <c r="W105" s="8" t="n">
         <v>50176</v>
       </c>
-      <c r="X105" s="8" t="n">
+      <c r="X105" s="8" t="n"/>
+      <c r="Y105" s="8" t="n"/>
+      <c r="Z105" s="8" t="n">
         <v>50176</v>
       </c>
     </row>
@@ -6563,6 +6792,8 @@
       <c r="X106" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y106" s="8" t="n"/>
+      <c r="Z106" s="8" t="n"/>
     </row>
     <row r="107">
       <c r="A107" s="7" t="n">
@@ -6614,9 +6845,11 @@
         <v>401408</v>
       </c>
       <c r="W107" s="8" t="n"/>
-      <c r="X107" s="8" t="n">
+      <c r="X107" s="8" t="n"/>
+      <c r="Y107" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="Z107" s="8" t="n"/>
     </row>
     <row r="108">
       <c r="A108" s="7" t="n">
@@ -6666,7 +6899,9 @@
       <c r="W108" s="8" t="n">
         <v>200704</v>
       </c>
-      <c r="X108" s="8" t="n">
+      <c r="X108" s="8" t="n"/>
+      <c r="Y108" s="8" t="n"/>
+      <c r="Z108" s="8" t="n">
         <v>200704</v>
       </c>
     </row>
@@ -6719,6 +6954,8 @@
       <c r="V109" s="8" t="n"/>
       <c r="W109" s="8" t="n"/>
       <c r="X109" s="8" t="n"/>
+      <c r="Y109" s="8" t="n"/>
+      <c r="Z109" s="8" t="n"/>
     </row>
     <row r="110">
       <c r="A110" s="7" t="n">
@@ -6785,6 +7022,8 @@
       <c r="X110" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y110" s="8" t="n"/>
+      <c r="Z110" s="8" t="n"/>
     </row>
     <row r="111">
       <c r="A111" s="7" t="n">
@@ -6836,9 +7075,11 @@
         <v>100352</v>
       </c>
       <c r="W111" s="8" t="n"/>
-      <c r="X111" s="8" t="n">
+      <c r="X111" s="8" t="n"/>
+      <c r="Y111" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="Z111" s="8" t="n"/>
     </row>
     <row r="112">
       <c r="A112" s="7" t="n">
@@ -6888,7 +7129,9 @@
       <c r="W112" s="8" t="n">
         <v>50176</v>
       </c>
-      <c r="X112" s="8" t="n">
+      <c r="X112" s="8" t="n"/>
+      <c r="Y112" s="8" t="n"/>
+      <c r="Z112" s="8" t="n">
         <v>50176</v>
       </c>
     </row>
@@ -6957,6 +7200,8 @@
       <c r="X113" s="8" t="n">
         <v>115605504</v>
       </c>
+      <c r="Y113" s="8" t="n"/>
+      <c r="Z113" s="8" t="n"/>
     </row>
     <row r="114">
       <c r="A114" s="7" t="n">
@@ -7008,9 +7253,11 @@
         <v>100352</v>
       </c>
       <c r="W114" s="8" t="n"/>
-      <c r="X114" s="8" t="n">
+      <c r="X114" s="8" t="n"/>
+      <c r="Y114" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="Z114" s="8" t="n"/>
     </row>
     <row r="115">
       <c r="A115" s="7" t="n">
@@ -7060,7 +7307,9 @@
       <c r="W115" s="8" t="n">
         <v>50176</v>
       </c>
-      <c r="X115" s="8" t="n">
+      <c r="X115" s="8" t="n"/>
+      <c r="Y115" s="8" t="n"/>
+      <c r="Z115" s="8" t="n">
         <v>50176</v>
       </c>
     </row>
@@ -7129,6 +7378,8 @@
       <c r="X116" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y116" s="8" t="n"/>
+      <c r="Z116" s="8" t="n"/>
     </row>
     <row r="117">
       <c r="A117" s="7" t="n">
@@ -7180,9 +7431,11 @@
         <v>401408</v>
       </c>
       <c r="W117" s="8" t="n"/>
-      <c r="X117" s="8" t="n">
+      <c r="X117" s="8" t="n"/>
+      <c r="Y117" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="Z117" s="8" t="n"/>
     </row>
     <row r="118">
       <c r="A118" s="7" t="n">
@@ -7232,7 +7485,9 @@
       <c r="W118" s="8" t="n">
         <v>200704</v>
       </c>
-      <c r="X118" s="8" t="n">
+      <c r="X118" s="8" t="n"/>
+      <c r="Y118" s="8" t="n"/>
+      <c r="Z118" s="8" t="n">
         <v>200704</v>
       </c>
     </row>
@@ -7285,6 +7540,8 @@
       <c r="V119" s="8" t="n"/>
       <c r="W119" s="8" t="n"/>
       <c r="X119" s="8" t="n"/>
+      <c r="Y119" s="8" t="n"/>
+      <c r="Z119" s="8" t="n"/>
     </row>
     <row r="120">
       <c r="A120" s="7" t="n">
@@ -7351,6 +7608,8 @@
       <c r="X120" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y120" s="8" t="n"/>
+      <c r="Z120" s="8" t="n"/>
     </row>
     <row r="121">
       <c r="A121" s="7" t="n">
@@ -7402,9 +7661,11 @@
         <v>100352</v>
       </c>
       <c r="W121" s="8" t="n"/>
-      <c r="X121" s="8" t="n">
+      <c r="X121" s="8" t="n"/>
+      <c r="Y121" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="Z121" s="8" t="n"/>
     </row>
     <row r="122">
       <c r="A122" s="7" t="n">
@@ -7454,7 +7715,9 @@
       <c r="W122" s="8" t="n">
         <v>50176</v>
       </c>
-      <c r="X122" s="8" t="n">
+      <c r="X122" s="8" t="n"/>
+      <c r="Y122" s="8" t="n"/>
+      <c r="Z122" s="8" t="n">
         <v>50176</v>
       </c>
     </row>
@@ -7523,6 +7786,8 @@
       <c r="X123" s="8" t="n">
         <v>115605504</v>
       </c>
+      <c r="Y123" s="8" t="n"/>
+      <c r="Z123" s="8" t="n"/>
     </row>
     <row r="124">
       <c r="A124" s="7" t="n">
@@ -7574,9 +7839,11 @@
         <v>100352</v>
       </c>
       <c r="W124" s="8" t="n"/>
-      <c r="X124" s="8" t="n">
+      <c r="X124" s="8" t="n"/>
+      <c r="Y124" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="Z124" s="8" t="n"/>
     </row>
     <row r="125">
       <c r="A125" s="7" t="n">
@@ -7626,7 +7893,9 @@
       <c r="W125" s="8" t="n">
         <v>50176</v>
       </c>
-      <c r="X125" s="8" t="n">
+      <c r="X125" s="8" t="n"/>
+      <c r="Y125" s="8" t="n"/>
+      <c r="Z125" s="8" t="n">
         <v>50176</v>
       </c>
     </row>
@@ -7695,6 +7964,8 @@
       <c r="X126" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y126" s="8" t="n"/>
+      <c r="Z126" s="8" t="n"/>
     </row>
     <row r="127">
       <c r="A127" s="7" t="n">
@@ -7746,9 +8017,11 @@
         <v>401408</v>
       </c>
       <c r="W127" s="8" t="n"/>
-      <c r="X127" s="8" t="n">
+      <c r="X127" s="8" t="n"/>
+      <c r="Y127" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="Z127" s="8" t="n"/>
     </row>
     <row r="128">
       <c r="A128" s="7" t="n">
@@ -7798,7 +8071,9 @@
       <c r="W128" s="8" t="n">
         <v>200704</v>
       </c>
-      <c r="X128" s="8" t="n">
+      <c r="X128" s="8" t="n"/>
+      <c r="Y128" s="8" t="n"/>
+      <c r="Z128" s="8" t="n">
         <v>200704</v>
       </c>
     </row>
@@ -7851,6 +8126,8 @@
       <c r="V129" s="8" t="n"/>
       <c r="W129" s="8" t="n"/>
       <c r="X129" s="8" t="n"/>
+      <c r="Y129" s="8" t="n"/>
+      <c r="Z129" s="8" t="n"/>
     </row>
     <row r="130">
       <c r="A130" s="7" t="n">
@@ -7917,6 +8194,8 @@
       <c r="X130" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y130" s="8" t="n"/>
+      <c r="Z130" s="8" t="n"/>
     </row>
     <row r="131">
       <c r="A131" s="7" t="n">
@@ -7968,9 +8247,11 @@
         <v>100352</v>
       </c>
       <c r="W131" s="8" t="n"/>
-      <c r="X131" s="8" t="n">
+      <c r="X131" s="8" t="n"/>
+      <c r="Y131" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="Z131" s="8" t="n"/>
     </row>
     <row r="132">
       <c r="A132" s="7" t="n">
@@ -8020,7 +8301,9 @@
       <c r="W132" s="8" t="n">
         <v>50176</v>
       </c>
-      <c r="X132" s="8" t="n">
+      <c r="X132" s="8" t="n"/>
+      <c r="Y132" s="8" t="n"/>
+      <c r="Z132" s="8" t="n">
         <v>50176</v>
       </c>
     </row>
@@ -8089,6 +8372,8 @@
       <c r="X133" s="8" t="n">
         <v>115605504</v>
       </c>
+      <c r="Y133" s="8" t="n"/>
+      <c r="Z133" s="8" t="n"/>
     </row>
     <row r="134">
       <c r="A134" s="7" t="n">
@@ -8140,9 +8425,11 @@
         <v>100352</v>
       </c>
       <c r="W134" s="8" t="n"/>
-      <c r="X134" s="8" t="n">
+      <c r="X134" s="8" t="n"/>
+      <c r="Y134" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="Z134" s="8" t="n"/>
     </row>
     <row r="135">
       <c r="A135" s="7" t="n">
@@ -8192,7 +8479,9 @@
       <c r="W135" s="8" t="n">
         <v>50176</v>
       </c>
-      <c r="X135" s="8" t="n">
+      <c r="X135" s="8" t="n"/>
+      <c r="Y135" s="8" t="n"/>
+      <c r="Z135" s="8" t="n">
         <v>50176</v>
       </c>
     </row>
@@ -8261,6 +8550,8 @@
       <c r="X136" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y136" s="8" t="n"/>
+      <c r="Z136" s="8" t="n"/>
     </row>
     <row r="137">
       <c r="A137" s="7" t="n">
@@ -8312,9 +8603,11 @@
         <v>401408</v>
       </c>
       <c r="W137" s="8" t="n"/>
-      <c r="X137" s="8" t="n">
+      <c r="X137" s="8" t="n"/>
+      <c r="Y137" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="Z137" s="8" t="n"/>
     </row>
     <row r="138">
       <c r="A138" s="7" t="n">
@@ -8364,7 +8657,9 @@
       <c r="W138" s="8" t="n">
         <v>200704</v>
       </c>
-      <c r="X138" s="8" t="n">
+      <c r="X138" s="8" t="n"/>
+      <c r="Y138" s="8" t="n"/>
+      <c r="Z138" s="8" t="n">
         <v>200704</v>
       </c>
     </row>
@@ -8417,6 +8712,8 @@
       <c r="V139" s="8" t="n"/>
       <c r="W139" s="8" t="n"/>
       <c r="X139" s="8" t="n"/>
+      <c r="Y139" s="8" t="n"/>
+      <c r="Z139" s="8" t="n"/>
     </row>
     <row r="140">
       <c r="A140" s="7" t="n">
@@ -8483,6 +8780,8 @@
       <c r="X140" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y140" s="8" t="n"/>
+      <c r="Z140" s="8" t="n"/>
     </row>
     <row r="141">
       <c r="A141" s="7" t="n">
@@ -8534,9 +8833,11 @@
         <v>100352</v>
       </c>
       <c r="W141" s="8" t="n"/>
-      <c r="X141" s="8" t="n">
+      <c r="X141" s="8" t="n"/>
+      <c r="Y141" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="Z141" s="8" t="n"/>
     </row>
     <row r="142">
       <c r="A142" s="7" t="n">
@@ -8586,7 +8887,9 @@
       <c r="W142" s="8" t="n">
         <v>50176</v>
       </c>
-      <c r="X142" s="8" t="n">
+      <c r="X142" s="8" t="n"/>
+      <c r="Y142" s="8" t="n"/>
+      <c r="Z142" s="8" t="n">
         <v>50176</v>
       </c>
     </row>
@@ -8655,6 +8958,8 @@
       <c r="X143" s="8" t="n">
         <v>115605504</v>
       </c>
+      <c r="Y143" s="8" t="n"/>
+      <c r="Z143" s="8" t="n"/>
     </row>
     <row r="144">
       <c r="A144" s="7" t="n">
@@ -8706,9 +9011,11 @@
         <v>100352</v>
       </c>
       <c r="W144" s="8" t="n"/>
-      <c r="X144" s="8" t="n">
+      <c r="X144" s="8" t="n"/>
+      <c r="Y144" s="8" t="n">
         <v>100352</v>
       </c>
+      <c r="Z144" s="8" t="n"/>
     </row>
     <row r="145">
       <c r="A145" s="7" t="n">
@@ -8758,7 +9065,9 @@
       <c r="W145" s="8" t="n">
         <v>50176</v>
       </c>
-      <c r="X145" s="8" t="n">
+      <c r="X145" s="8" t="n"/>
+      <c r="Y145" s="8" t="n"/>
+      <c r="Z145" s="8" t="n">
         <v>50176</v>
       </c>
     </row>
@@ -8827,6 +9136,8 @@
       <c r="X146" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y146" s="8" t="n"/>
+      <c r="Z146" s="8" t="n"/>
     </row>
     <row r="147">
       <c r="A147" s="7" t="n">
@@ -8878,9 +9189,11 @@
         <v>401408</v>
       </c>
       <c r="W147" s="8" t="n"/>
-      <c r="X147" s="8" t="n">
+      <c r="X147" s="8" t="n"/>
+      <c r="Y147" s="8" t="n">
         <v>401408</v>
       </c>
+      <c r="Z147" s="8" t="n"/>
     </row>
     <row r="148">
       <c r="A148" s="7" t="n">
@@ -8930,7 +9243,9 @@
       <c r="W148" s="8" t="n">
         <v>200704</v>
       </c>
-      <c r="X148" s="8" t="n">
+      <c r="X148" s="8" t="n"/>
+      <c r="Y148" s="8" t="n"/>
+      <c r="Z148" s="8" t="n">
         <v>200704</v>
       </c>
     </row>
@@ -8981,6 +9296,8 @@
       <c r="V149" s="8" t="n"/>
       <c r="W149" s="8" t="n"/>
       <c r="X149" s="8" t="n"/>
+      <c r="Y149" s="8" t="n"/>
+      <c r="Z149" s="8" t="n"/>
     </row>
     <row r="150">
       <c r="A150" s="7" t="n">
@@ -9031,6 +9348,8 @@
       <c r="V150" s="8" t="n"/>
       <c r="W150" s="8" t="n"/>
       <c r="X150" s="8" t="n"/>
+      <c r="Y150" s="8" t="n"/>
+      <c r="Z150" s="8" t="n"/>
     </row>
     <row r="151">
       <c r="A151" s="7" t="n">
@@ -9097,6 +9416,8 @@
       <c r="X151" s="8" t="n">
         <v>102760448</v>
       </c>
+      <c r="Y151" s="8" t="n"/>
+      <c r="Z151" s="8" t="n"/>
     </row>
     <row r="152">
       <c r="A152" s="7" t="n">
@@ -9148,9 +9469,11 @@
         <v>200704</v>
       </c>
       <c r="W152" s="8" t="n"/>
-      <c r="X152" s="8" t="n">
-        <v>200704</v>
-      </c>
+      <c r="X152" s="8" t="n"/>
+      <c r="Y152" s="8" t="n">
+        <v>200704</v>
+      </c>
+      <c r="Z152" s="8" t="n"/>
     </row>
     <row r="153">
       <c r="A153" s="7" t="n">
@@ -9200,7 +9523,9 @@
       <c r="W153" s="8" t="n">
         <v>100352</v>
       </c>
-      <c r="X153" s="8" t="n">
+      <c r="X153" s="8" t="n"/>
+      <c r="Y153" s="8" t="n"/>
+      <c r="Z153" s="8" t="n">
         <v>100352</v>
       </c>
     </row>
@@ -9262,13 +9587,15 @@
         <v>2359296</v>
       </c>
       <c r="U154" s="8" t="n">
-        <v>462422016</v>
+        <v>115605504</v>
       </c>
       <c r="V154" s="8" t="n"/>
       <c r="W154" s="8" t="n"/>
       <c r="X154" s="8" t="n">
         <v>462422016</v>
       </c>
+      <c r="Y154" s="8" t="n"/>
+      <c r="Z154" s="8" t="n"/>
     </row>
     <row r="155">
       <c r="A155" s="7" t="n">
@@ -9320,9 +9647,11 @@
         <v>50176</v>
       </c>
       <c r="W155" s="8" t="n"/>
-      <c r="X155" s="8" t="n">
+      <c r="X155" s="8" t="n"/>
+      <c r="Y155" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="Z155" s="8" t="n"/>
     </row>
     <row r="156">
       <c r="A156" s="7" t="n">
@@ -9372,7 +9701,9 @@
       <c r="W156" s="8" t="n">
         <v>25088</v>
       </c>
-      <c r="X156" s="8" t="n">
+      <c r="X156" s="8" t="n"/>
+      <c r="Y156" s="8" t="n"/>
+      <c r="Z156" s="8" t="n">
         <v>25088</v>
       </c>
     </row>
@@ -9441,6 +9772,8 @@
       <c r="X157" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y157" s="8" t="n"/>
+      <c r="Z157" s="8" t="n"/>
     </row>
     <row r="158">
       <c r="A158" s="7" t="n">
@@ -9492,9 +9825,11 @@
         <v>200704</v>
       </c>
       <c r="W158" s="8" t="n"/>
-      <c r="X158" s="8" t="n">
-        <v>200704</v>
-      </c>
+      <c r="X158" s="8" t="n"/>
+      <c r="Y158" s="8" t="n">
+        <v>200704</v>
+      </c>
+      <c r="Z158" s="8" t="n"/>
     </row>
     <row r="159">
       <c r="A159" s="7" t="n">
@@ -9543,6 +9878,8 @@
       <c r="V159" s="8" t="n"/>
       <c r="W159" s="8" t="n"/>
       <c r="X159" s="8" t="n"/>
+      <c r="Y159" s="8" t="n"/>
+      <c r="Z159" s="8" t="n"/>
     </row>
     <row r="160">
       <c r="A160" s="7" t="n">
@@ -9602,13 +9939,15 @@
         <v>2097152</v>
       </c>
       <c r="U160" s="8" t="n">
-        <v>411041792</v>
+        <v>102760448</v>
       </c>
       <c r="V160" s="8" t="n"/>
       <c r="W160" s="8" t="n"/>
       <c r="X160" s="8" t="n">
         <v>411041792</v>
       </c>
+      <c r="Y160" s="8" t="n"/>
+      <c r="Z160" s="8" t="n"/>
     </row>
     <row r="161">
       <c r="A161" s="7" t="n">
@@ -9660,9 +9999,11 @@
         <v>200704</v>
       </c>
       <c r="W161" s="8" t="n"/>
-      <c r="X161" s="8" t="n">
-        <v>200704</v>
-      </c>
+      <c r="X161" s="8" t="n"/>
+      <c r="Y161" s="8" t="n">
+        <v>200704</v>
+      </c>
+      <c r="Z161" s="8" t="n"/>
     </row>
     <row r="162">
       <c r="A162" s="7" t="n">
@@ -9712,7 +10053,9 @@
       <c r="W162" s="8" t="n">
         <v>100352</v>
       </c>
-      <c r="X162" s="8" t="n">
+      <c r="X162" s="8" t="n"/>
+      <c r="Y162" s="8" t="n"/>
+      <c r="Z162" s="8" t="n">
         <v>100352</v>
       </c>
     </row>
@@ -9765,6 +10108,8 @@
       <c r="V163" s="8" t="n"/>
       <c r="W163" s="8" t="n"/>
       <c r="X163" s="8" t="n"/>
+      <c r="Y163" s="8" t="n"/>
+      <c r="Z163" s="8" t="n"/>
     </row>
     <row r="164">
       <c r="A164" s="7" t="n">
@@ -9831,6 +10176,8 @@
       <c r="X164" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y164" s="8" t="n"/>
+      <c r="Z164" s="8" t="n"/>
     </row>
     <row r="165">
       <c r="A165" s="7" t="n">
@@ -9882,9 +10229,11 @@
         <v>50176</v>
       </c>
       <c r="W165" s="8" t="n"/>
-      <c r="X165" s="8" t="n">
+      <c r="X165" s="8" t="n"/>
+      <c r="Y165" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="Z165" s="8" t="n"/>
     </row>
     <row r="166">
       <c r="A166" s="7" t="n">
@@ -9934,7 +10283,9 @@
       <c r="W166" s="8" t="n">
         <v>25088</v>
       </c>
-      <c r="X166" s="8" t="n">
+      <c r="X166" s="8" t="n"/>
+      <c r="Y166" s="8" t="n"/>
+      <c r="Z166" s="8" t="n">
         <v>25088</v>
       </c>
     </row>
@@ -10003,6 +10354,8 @@
       <c r="X167" s="8" t="n">
         <v>115605504</v>
       </c>
+      <c r="Y167" s="8" t="n"/>
+      <c r="Z167" s="8" t="n"/>
     </row>
     <row r="168">
       <c r="A168" s="7" t="n">
@@ -10054,9 +10407,11 @@
         <v>50176</v>
       </c>
       <c r="W168" s="8" t="n"/>
-      <c r="X168" s="8" t="n">
+      <c r="X168" s="8" t="n"/>
+      <c r="Y168" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="Z168" s="8" t="n"/>
     </row>
     <row r="169">
       <c r="A169" s="7" t="n">
@@ -10106,7 +10461,9 @@
       <c r="W169" s="8" t="n">
         <v>25088</v>
       </c>
-      <c r="X169" s="8" t="n">
+      <c r="X169" s="8" t="n"/>
+      <c r="Y169" s="8" t="n"/>
+      <c r="Z169" s="8" t="n">
         <v>25088</v>
       </c>
     </row>
@@ -10175,6 +10532,8 @@
       <c r="X170" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y170" s="8" t="n"/>
+      <c r="Z170" s="8" t="n"/>
     </row>
     <row r="171">
       <c r="A171" s="7" t="n">
@@ -10226,9 +10585,11 @@
         <v>200704</v>
       </c>
       <c r="W171" s="8" t="n"/>
-      <c r="X171" s="8" t="n">
-        <v>200704</v>
-      </c>
+      <c r="X171" s="8" t="n"/>
+      <c r="Y171" s="8" t="n">
+        <v>200704</v>
+      </c>
+      <c r="Z171" s="8" t="n"/>
     </row>
     <row r="172">
       <c r="A172" s="7" t="n">
@@ -10278,7 +10639,9 @@
       <c r="W172" s="8" t="n">
         <v>100352</v>
       </c>
-      <c r="X172" s="8" t="n">
+      <c r="X172" s="8" t="n"/>
+      <c r="Y172" s="8" t="n"/>
+      <c r="Z172" s="8" t="n">
         <v>100352</v>
       </c>
     </row>
@@ -10331,6 +10694,8 @@
       <c r="V173" s="8" t="n"/>
       <c r="W173" s="8" t="n"/>
       <c r="X173" s="8" t="n"/>
+      <c r="Y173" s="8" t="n"/>
+      <c r="Z173" s="8" t="n"/>
     </row>
     <row r="174">
       <c r="A174" s="7" t="n">
@@ -10397,6 +10762,8 @@
       <c r="X174" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y174" s="8" t="n"/>
+      <c r="Z174" s="8" t="n"/>
     </row>
     <row r="175">
       <c r="A175" s="7" t="n">
@@ -10448,9 +10815,11 @@
         <v>50176</v>
       </c>
       <c r="W175" s="8" t="n"/>
-      <c r="X175" s="8" t="n">
+      <c r="X175" s="8" t="n"/>
+      <c r="Y175" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="Z175" s="8" t="n"/>
     </row>
     <row r="176">
       <c r="A176" s="7" t="n">
@@ -10500,7 +10869,9 @@
       <c r="W176" s="8" t="n">
         <v>25088</v>
       </c>
-      <c r="X176" s="8" t="n">
+      <c r="X176" s="8" t="n"/>
+      <c r="Y176" s="8" t="n"/>
+      <c r="Z176" s="8" t="n">
         <v>25088</v>
       </c>
     </row>
@@ -10569,6 +10940,8 @@
       <c r="X177" s="8" t="n">
         <v>115605504</v>
       </c>
+      <c r="Y177" s="8" t="n"/>
+      <c r="Z177" s="8" t="n"/>
     </row>
     <row r="178">
       <c r="A178" s="7" t="n">
@@ -10620,9 +10993,11 @@
         <v>50176</v>
       </c>
       <c r="W178" s="8" t="n"/>
-      <c r="X178" s="8" t="n">
+      <c r="X178" s="8" t="n"/>
+      <c r="Y178" s="8" t="n">
         <v>50176</v>
       </c>
+      <c r="Z178" s="8" t="n"/>
     </row>
     <row r="179">
       <c r="A179" s="7" t="n">
@@ -10672,7 +11047,9 @@
       <c r="W179" s="8" t="n">
         <v>25088</v>
       </c>
-      <c r="X179" s="8" t="n">
+      <c r="X179" s="8" t="n"/>
+      <c r="Y179" s="8" t="n"/>
+      <c r="Z179" s="8" t="n">
         <v>25088</v>
       </c>
     </row>
@@ -10741,6 +11118,8 @@
       <c r="X180" s="8" t="n">
         <v>51380224</v>
       </c>
+      <c r="Y180" s="8" t="n"/>
+      <c r="Z180" s="8" t="n"/>
     </row>
     <row r="181">
       <c r="A181" s="7" t="n">
@@ -10792,9 +11171,11 @@
         <v>200704</v>
       </c>
       <c r="W181" s="8" t="n"/>
-      <c r="X181" s="8" t="n">
-        <v>200704</v>
-      </c>
+      <c r="X181" s="8" t="n"/>
+      <c r="Y181" s="8" t="n">
+        <v>200704</v>
+      </c>
+      <c r="Z181" s="8" t="n"/>
     </row>
     <row r="182">
       <c r="A182" s="7" t="n">
@@ -10844,7 +11225,9 @@
       <c r="W182" s="8" t="n">
         <v>100352</v>
       </c>
-      <c r="X182" s="8" t="n">
+      <c r="X182" s="8" t="n"/>
+      <c r="Y182" s="8" t="n"/>
+      <c r="Z182" s="8" t="n">
         <v>100352</v>
       </c>
     </row>
@@ -10895,6 +11278,8 @@
       <c r="V183" s="8" t="n"/>
       <c r="W183" s="8" t="n"/>
       <c r="X183" s="8" t="n"/>
+      <c r="Y183" s="8" t="n"/>
+      <c r="Z183" s="8" t="n"/>
     </row>
     <row r="184">
       <c r="A184" s="7" t="n">
@@ -10941,9 +11326,11 @@
       <c r="X184" s="8" t="n">
         <v>2048000</v>
       </c>
+      <c r="Y184" s="8" t="n"/>
+      <c r="Z184" s="8" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
@@ -10951,7 +11338,8 @@
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:T1"/>
-    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="X1:Z1"/>
   </mergeCells>
   <conditionalFormatting sqref="S1:S184">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
@@ -10965,6 +11353,11 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U184">
     <cfRule type="cellIs" priority="3" operator="equal" dxfId="2" stopIfTrue="1">
+      <formula>118013952</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X1:X184">
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3" stopIfTrue="1">
       <formula>472055808</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10978,7 +11371,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11020,10 +11413,20 @@
     <row r="4">
       <c r="A4" s="8" t="inlineStr">
         <is>
-          <t>Total GEMM (G_ops):</t>
+          <t>Total Forward GEMM (G_ops):</t>
         </is>
       </c>
       <c r="B4" s="8" t="n">
+        <v>4.089184256</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="inlineStr">
+        <is>
+          <t>Total Backward GEMM (G_ops):</t>
+        </is>
+      </c>
+      <c r="B5" s="8" t="n">
         <v>6.40851968</v>
       </c>
     </row>

</xml_diff>